<commit_message>
mis en place d un bout de modele
</commit_message>
<xml_diff>
--- a/annexe/Modèle investissement.xlsx
+++ b/annexe/Modèle investissement.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDAC2E0-BE4E-4A67-B3C1-CDD38C369118}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45F6C0B-5E22-4BA2-83C0-DBCE551B20CB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="2" r:id="rId1"/>
@@ -2481,38 +2481,38 @@
     <xf numFmtId="164" fontId="0" fillId="45" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2897,7 +2897,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2922,19 +2922,19 @@
       <c r="B3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="216" t="s">
+      <c r="E3" s="214" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="217"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="214" t="s">
+      <c r="F3" s="215"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="212" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="215"/>
-      <c r="J3" s="214" t="s">
+      <c r="I3" s="213"/>
+      <c r="J3" s="212" t="s">
         <v>326</v>
       </c>
-      <c r="K3" s="215"/>
+      <c r="K3" s="213"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D4" s="190"/>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="E5" s="194">
         <f>Select!C68</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F5" s="195" t="str">
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(Select!F68&lt;&gt;"",Select!F68,IF(Select!G68&lt;&gt;"",(100%-Select!G68)*Select!C68,"")))</f>
@@ -2986,11 +2986,11 @@
       </c>
       <c r="H5" s="197">
         <f>Modèle!D163</f>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="I5" s="198">
         <f>Modèle!I163</f>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911436E-2</v>
       </c>
       <c r="J5" s="208"/>
       <c r="K5" s="209"/>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="E6" s="201">
         <f>Select!C69</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F6" s="203" t="str">
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(Select!F69&lt;&gt;"",Select!F69,IF(Select!G69&lt;&gt;"",(100%-Select!G69)*Select!C69,"")))</f>
@@ -3012,21 +3012,21 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F69&lt;&gt;"",Select!G69&lt;&gt;""),Select!E69,""))</f>
         <v/>
       </c>
-      <c r="H6" s="219">
+      <c r="H6" s="217">
         <f>Modèle!D164</f>
-        <v>0.27174915611814349</v>
-      </c>
-      <c r="I6" s="221">
+        <v>0.2075443037974681</v>
+      </c>
+      <c r="I6" s="219">
         <f>Modèle!I164</f>
-        <v>0.27698511809808679</v>
-      </c>
-      <c r="J6" s="219">
+        <v>0.23575416816926681</v>
+      </c>
+      <c r="J6" s="217">
         <f>Modèle!D192</f>
         <v>0</v>
       </c>
-      <c r="K6" s="221">
+      <c r="K6" s="219">
         <f>Modèle!H192</f>
-        <v>0.73717564368863553</v>
+        <v>0.62149337538873961</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3035,7 +3035,7 @@
         <v>Pays</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D7" s="200" t="str">
         <f>VLOOKUP(CONCATENATE(_Impot,_Impot_IMF),_Tables,3,FALSE)</f>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="E7" s="202">
         <f>Select!C70</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F7" s="206" t="str">
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(Select!F70&lt;&gt;"",Select!F70,IF(Select!G70&lt;&gt;"",(100%-Select!G70)*Select!C70,"")))</f>
@@ -3053,10 +3053,10 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F70&lt;&gt;"",Select!G70&lt;&gt;""),Select!E70,""))</f>
         <v/>
       </c>
-      <c r="H7" s="220"/>
-      <c r="I7" s="222"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="222"/>
+      <c r="H7" s="218"/>
+      <c r="I7" s="220"/>
+      <c r="J7" s="218"/>
+      <c r="K7" s="220"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="56" t="str">
@@ -3065,7 +3065,7 @@
       </c>
       <c r="E8" s="194">
         <f>Select!C71</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="195" t="str">
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(Select!F71&lt;&gt;"",Select!F71,IF(Select!G71&lt;&gt;"",(100%-Select!G71)*Select!C71,"")))</f>
@@ -3077,11 +3077,11 @@
       </c>
       <c r="H8" s="197">
         <f>Modèle!D165</f>
-        <v>7.7642616033755302E-2</v>
+        <v>3.4590717299578015E-2</v>
       </c>
       <c r="I8" s="198">
         <f>Modèle!I165</f>
-        <v>7.9138605170881962E-2</v>
+        <v>3.9292361361544466E-2</v>
       </c>
       <c r="J8" s="208"/>
       <c r="K8" s="209"/>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="E9" s="183">
         <f>Select!C72</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F9" s="80" t="str">
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(Select!F72&lt;&gt;"",Select!F72,IF(Select!G72&lt;&gt;"",(100%-Select!G72)*Select!C72,"")))</f>
@@ -3112,11 +3112,11 @@
       </c>
       <c r="H9" s="188">
         <f>Modèle!D166</f>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="I9" s="172">
         <f>Modèle!I166</f>
-        <v>1.3924050632911395E-2</v>
+        <v>1.0443037974683558E-2</v>
       </c>
       <c r="J9" s="210"/>
       <c r="K9" s="211"/>
@@ -3166,11 +3166,11 @@
       <c r="G11" s="52"/>
       <c r="H11" s="189">
         <f>Modèle!D168</f>
-        <v>0.43710063291139256</v>
+        <v>0.28650210970464107</v>
       </c>
       <c r="I11" s="174">
         <f>Modèle!I168</f>
-        <v>0.44383258402846243</v>
+        <v>0.31941361813840624</v>
       </c>
       <c r="J11" s="189">
         <f>Modèle!D195</f>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="K11" s="174">
         <f>Modèle!H195</f>
-        <v>1</v>
+        <v>0.86390257497952883</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -3193,15 +3193,15 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="212" t="str">
+      <c r="A16" s="221" t="str">
         <f>VLOOKUP(_Bilan,_Tables,4,FALSE)</f>
         <v>Bilan à l'ouverture</v>
       </c>
-      <c r="B16" s="212"/>
-      <c r="C16" s="212"/>
-      <c r="D16" s="212"/>
-      <c r="E16" s="212"/>
-      <c r="F16" s="212"/>
+      <c r="B16" s="221"/>
+      <c r="C16" s="221"/>
+      <c r="D16" s="221"/>
+      <c r="E16" s="221"/>
+      <c r="F16" s="221"/>
       <c r="H16" s="73" t="str">
         <f>VLOOKUP(_PIBPNB,_Tables,4,FALSE)</f>
         <v>PIB ou PNB</v>
@@ -3211,18 +3211,18 @@
       <c r="K16" s="68"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="213" t="str">
+      <c r="A17" s="222" t="str">
         <f>VLOOKUP(_Actif,_Tables,4,FALSE)</f>
         <v>Actif</v>
       </c>
-      <c r="B17" s="213"/>
-      <c r="C17" s="213"/>
-      <c r="D17" s="213" t="str">
+      <c r="B17" s="222"/>
+      <c r="C17" s="222"/>
+      <c r="D17" s="222" t="str">
         <f>VLOOKUP(_Passif,_Tables,4,FALSE)</f>
         <v>Passif</v>
       </c>
-      <c r="E17" s="213"/>
-      <c r="F17" s="213"/>
+      <c r="E17" s="222"/>
+      <c r="F17" s="222"/>
       <c r="H17" s="56" t="str">
         <f>_PIBPNB_Liste</f>
         <v>PIB/tête</v>
@@ -3230,7 +3230,7 @@
       <c r="I17" s="57"/>
       <c r="J17" s="69">
         <f>_PIBPNB_Select</f>
-        <v>506611.40425374068</v>
+        <v>446686.61040326342</v>
       </c>
       <c r="K17" s="70" t="s">
         <v>251</v>
@@ -3527,29 +3527,29 @@
       <c r="K29" s="70"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="212" t="str">
+      <c r="A31" s="221" t="str">
         <f>VLOOKUP(_CompteDeResultat,_Tables,4,FALSE)</f>
         <v>Compte de résultat</v>
       </c>
-      <c r="B31" s="212"/>
-      <c r="C31" s="212"/>
-      <c r="D31" s="212"/>
-      <c r="E31" s="212"/>
-      <c r="F31" s="212"/>
+      <c r="B31" s="221"/>
+      <c r="C31" s="221"/>
+      <c r="D31" s="221"/>
+      <c r="E31" s="221"/>
+      <c r="F31" s="221"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="213" t="str">
+      <c r="A32" s="222" t="str">
         <f>VLOOKUP(_Charges,_Tables,4,FALSE)</f>
         <v>Charges</v>
       </c>
-      <c r="B32" s="213"/>
-      <c r="C32" s="213"/>
-      <c r="D32" s="213" t="str">
+      <c r="B32" s="222"/>
+      <c r="C32" s="222"/>
+      <c r="D32" s="222" t="str">
         <f>VLOOKUP(_Produits,_Tables,4,FALSE)</f>
         <v>Produits</v>
       </c>
-      <c r="E32" s="213"/>
-      <c r="F32" s="213"/>
+      <c r="E32" s="222"/>
+      <c r="F32" s="222"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="str">
@@ -3799,23 +3799,23 @@
       </c>
       <c r="B52" s="80">
         <f>_CFE_Taux_Select1</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="C52" s="80">
         <f>_CFE_Taux_Select2</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D52" s="80">
         <f>_CFE_Taux_Select3</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E52" s="80">
         <f>_CFE_Taux_Select4</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F52" s="81">
         <f>_CFE_Taux_Select5</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H52" s="38" t="str">
         <f>VLOOKUP(_Constructions,_Tables,4,FALSE)</f>
@@ -3838,23 +3838,23 @@
       </c>
       <c r="B53" s="80">
         <f>_IS_Taux_Select1</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="C53" s="80">
         <f>_IS_Taux_Select2</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D53" s="80">
         <f>_IS_Taux_Select3</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E53" s="80">
         <f>_IS_Taux_Select4</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F53" s="81">
         <f>_IS_Taux_Select5</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="H53" s="38" t="str">
         <f>VLOOKUP(_Equipement,_Tables,4,FALSE)</f>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="K53" s="41">
         <f>_Equipement_CoefDegressif_Select</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -3877,23 +3877,23 @@
       </c>
       <c r="B54" s="80">
         <f>_IMF_Taux_Select1</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="C54" s="80">
         <f>_IMF_Taux_Select2</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="D54" s="80">
         <f>_IMF_Taux_Select3</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E54" s="80">
         <f>_IMF_Taux_Select4</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F54" s="81">
         <f>_IMF_Taux_Select5</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="H54" s="38" t="str">
         <f>VLOOKUP(_Camion,_Tables,4,FALSE)</f>
@@ -3916,23 +3916,23 @@
       </c>
       <c r="B55" s="80">
         <f>_IRVM_Taux_Select1</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C55" s="80">
         <f>_IRVM_Taux_Select2</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D55" s="80">
         <f>_IRVM_Taux_Select3</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E55" s="80">
         <f>_IRVM_Taux_Select4</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F55" s="81">
         <f>_IRVM_Taux_Select5</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H55" s="38" t="str">
         <f>VLOOKUP(_Informatique,_Tables,4,FALSE)</f>
@@ -3941,7 +3941,7 @@
       <c r="I55" s="39"/>
       <c r="J55" s="40">
         <f>_Informatique_DureeLineaire_Select</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K55" s="41">
         <f>_Informatique_CoefDegressif_Select</f>
@@ -3955,23 +3955,23 @@
       </c>
       <c r="B56" s="80">
         <f>_IRC_Taux_Select1</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C56" s="80">
         <f>_IRC_Taux_Select2</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D56" s="80">
         <f>_IRC_Taux_Select3</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E56" s="80">
         <f>_IRC_Taux_Select4</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F56" s="81">
         <f>_IRC_Taux_Select5</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="H56" s="45" t="str">
         <f>VLOOKUP(_Bureau,_Tables,4,FALSE)</f>
@@ -4065,6 +4065,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E3:G3"/>
@@ -4072,12 +4078,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4122,8 +4122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="G38" s="30">
         <f>VLOOKUP($B$38,_BaseFisc,_ColonneFisc_Select,FALSE)</f>
-        <v>506611.40425374068</v>
+        <v>446686.61040326342</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="G40" s="32">
         <f>IF(G39&lt;&gt;"",G39,G38)</f>
-        <v>506611.40425374068</v>
+        <v>446686.61040326342</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="B42" s="19" t="str">
         <f>VLOOKUP(1,$C43:$D54,2,FALSE)</f>
-        <v>_TCD</v>
+        <v>_BEN</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="C43" s="3">
         <f t="shared" ref="C43:C54" si="3">IF(_Pays_Liste=$B43,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3" t="str">
         <f>_Pays_BEN</f>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="C53" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="3" t="str">
         <f>_Pays_TCD</f>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="B56" s="19">
         <f>HLOOKUP(_Pays_Select,BaseFisc!$E$1:$R$2,2,FALSE)</f>
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="C68" s="12">
         <f>IF(VLOOKUP(CONCATENATE($C$66,$B68,C$67),_BaseFisc,_ColonneFisc_Select,FALSE)="","",VLOOKUP(CONCATENATE($C$66,$B68,C$67),_BaseFisc,_ColonneFisc_Select,FALSE))</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E68" s="23" t="str">
         <f t="shared" ref="E68:G73" si="4">IF(VLOOKUP(CONCATENATE($E$66,$B68,E$67),_BaseFisc,_ColonneFisc_Select,FALSE)="","",VLOOKUP(CONCATENATE($E$66,$B68,E$67),_BaseFisc,_ColonneFisc_Select,FALSE))</f>
@@ -5024,23 +5024,23 @@
       <c r="N68" s="25"/>
       <c r="P68" s="24">
         <f t="shared" ref="P68:T73" si="6">IF(J68&lt;&gt;"",J68,IF(OR(_Regime_Select=_Regime_Gen,$H68=_Regime_Gen),$C68,IF($E68&lt;P$67,$C68,IF($H68=_Information_Taux,$F68,IF($H68=_Information_ReducExo,(1-$G68)*$C68,_Error)))))</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="Q68" s="24">
         <f t="shared" si="6"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="R68" s="24">
         <f t="shared" si="6"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="S68" s="24">
         <f t="shared" si="6"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="T68" s="24">
         <f t="shared" si="6"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
@@ -5049,8 +5049,8 @@
         <v>_IS</v>
       </c>
       <c r="C69" s="12">
-        <f t="shared" ref="C68:C73" si="7">IF(VLOOKUP(CONCATENATE($C$66,$B69,C$67),_BaseFisc,_ColonneFisc_Select,FALSE)="","",VLOOKUP(CONCATENATE($C$66,$B69,C$67),_BaseFisc,_ColonneFisc_Select,FALSE))</f>
-        <v>0.35</v>
+        <f t="shared" ref="C69:C73" si="7">IF(VLOOKUP(CONCATENATE($C$66,$B69,C$67),_BaseFisc,_ColonneFisc_Select,FALSE)="","",VLOOKUP(CONCATENATE($C$66,$B69,C$67),_BaseFisc,_ColonneFisc_Select,FALSE))</f>
+        <v>0.3</v>
       </c>
       <c r="E69" s="23">
         <f>IF(VLOOKUP(CONCATENATE($E$66,$B69,E$67),_BaseFisc,_ColonneFisc_Select,FALSE)="","",VLOOKUP(CONCATENATE($E$66,$B69,E$67),_BaseFisc,_ColonneFisc_Select,FALSE))</f>
@@ -5075,23 +5075,23 @@
       <c r="N69" s="25"/>
       <c r="P69" s="24">
         <f t="shared" si="6"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="Q69" s="24">
         <f t="shared" si="6"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="R69" s="24">
         <f t="shared" si="6"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="S69" s="24">
         <f t="shared" si="6"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="T69" s="24">
         <f t="shared" si="6"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
@@ -5101,23 +5101,23 @@
       </c>
       <c r="C70" s="12">
         <f t="shared" si="7"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E70" s="23">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E70" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="F70" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="G70" s="10">
+      <c r="G70" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H70" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>_ReducExo</v>
+        <v>_Gen</v>
       </c>
       <c r="J70" s="25"/>
       <c r="K70" s="25"/>
@@ -5126,23 +5126,23 @@
       <c r="N70" s="25"/>
       <c r="P70" s="24">
         <f t="shared" si="6"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="Q70" s="24">
         <f t="shared" si="6"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="R70" s="24">
         <f t="shared" si="6"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="S70" s="24">
         <f t="shared" si="6"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="T70" s="24">
         <f t="shared" si="6"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="C71" s="12">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E71" s="23" t="str">
         <f t="shared" si="4"/>
@@ -5177,23 +5177,23 @@
       <c r="N71" s="25"/>
       <c r="P71" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="Q71" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="R71" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S71" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T71" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
@@ -5203,7 +5203,7 @@
       </c>
       <c r="C72" s="12">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E72" s="23" t="str">
         <f t="shared" si="4"/>
@@ -5228,23 +5228,23 @@
       <c r="N72" s="25"/>
       <c r="P72" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="Q72" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="R72" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="S72" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="T72" s="24">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="D78" s="23">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="27"/>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="J78" s="26">
         <f>IF(G78&lt;&gt;"",G78,IF(D78="",1,IF(D78&lt;1,_Error,D78)))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
@@ -5421,7 +5421,7 @@
       </c>
       <c r="C80" s="23">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80" s="23" t="str">
         <f t="shared" si="8"/>
@@ -5431,7 +5431,7 @@
       <c r="G80" s="27"/>
       <c r="I80" s="26">
         <f>IF(F80&lt;&gt;"",F80,IF(C80&lt;1,_Error,C80))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J80" s="26">
         <f>IF(G80&lt;&gt;"",G80,IF(D80="",1,IF(D80&lt;1,_Error,D80)))</f>
@@ -5566,7 +5566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D114"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7117,10 +7117,10 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9009,7 +9009,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9430,11 +9430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J195"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="C4" s="93">
         <f>(_Terrain_Select+_Constructions_Select+_Equipement_Select+_Camion_Select+_Informatique_Select+_Bureau_Select)*_PIBPNB_Select</f>
-        <v>73458653.616792396</v>
+        <v>64769558.508473195</v>
       </c>
       <c r="D4" s="91"/>
       <c r="E4" s="91"/>
@@ -9509,23 +9509,23 @@
       <c r="C7" s="116"/>
       <c r="D7" s="117">
         <f>D$22</f>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652684</v>
       </c>
       <c r="E7" s="117">
         <f t="shared" ref="E7:H7" si="0">E$22</f>
-        <v>1013222.8085074815</v>
+        <v>893373.2208065266</v>
       </c>
       <c r="F7" s="117">
         <f t="shared" si="0"/>
-        <v>1013222.8085074816</v>
+        <v>893373.22080652672</v>
       </c>
       <c r="G7" s="117">
         <f t="shared" si="0"/>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652672</v>
       </c>
       <c r="H7" s="118">
         <f t="shared" si="0"/>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652684</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -9538,23 +9538,23 @@
       <c r="C8" s="119"/>
       <c r="D8" s="113">
         <f>D$32</f>
-        <v>3039668.4255224443</v>
+        <v>6700299.1560489517</v>
       </c>
       <c r="E8" s="113">
         <f t="shared" ref="E8:H8" si="1">E$32</f>
-        <v>3039668.4255224438</v>
+        <v>5025224.3670367133</v>
       </c>
       <c r="F8" s="113">
         <f t="shared" si="1"/>
-        <v>3039668.4255224443</v>
+        <v>3768918.275277535</v>
       </c>
       <c r="G8" s="113">
         <f t="shared" si="1"/>
-        <v>3039668.4255224443</v>
+        <v>2826688.7064581513</v>
       </c>
       <c r="H8" s="120">
         <f t="shared" si="1"/>
-        <v>3039668.4255224448</v>
+        <v>2120016.5298436135</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -9567,15 +9567,15 @@
       <c r="C9" s="119"/>
       <c r="D9" s="113">
         <f>D$42</f>
-        <v>844352.34042290109</v>
+        <v>744477.68400543893</v>
       </c>
       <c r="E9" s="113">
         <f t="shared" ref="E9:H9" si="2">E$42</f>
-        <v>844352.34042290121</v>
+        <v>744477.68400543905</v>
       </c>
       <c r="F9" s="113">
         <f t="shared" si="2"/>
-        <v>844352.34042290121</v>
+        <v>744477.68400543905</v>
       </c>
       <c r="G9" s="113">
         <f t="shared" si="2"/>
@@ -9596,15 +9596,15 @@
       <c r="C10" s="119"/>
       <c r="D10" s="113">
         <f>D$52</f>
-        <v>844352.34042290109</v>
+        <v>1116716.5260081585</v>
       </c>
       <c r="E10" s="113">
         <f t="shared" ref="E10:H10" si="3">E$52</f>
-        <v>844352.34042290121</v>
+        <v>1116716.5260081585</v>
       </c>
       <c r="F10" s="113">
         <f t="shared" si="3"/>
-        <v>844352.34042290121</v>
+        <v>0</v>
       </c>
       <c r="G10" s="113">
         <f t="shared" si="3"/>
@@ -9625,23 +9625,23 @@
       <c r="C11" s="119"/>
       <c r="D11" s="113">
         <f>D$62</f>
-        <v>253305.70212687037</v>
+        <v>223343.30520163171</v>
       </c>
       <c r="E11" s="113">
         <f t="shared" ref="E11:H11" si="4">E$62</f>
-        <v>253305.70212687034</v>
+        <v>223343.30520163168</v>
       </c>
       <c r="F11" s="113">
         <f t="shared" si="4"/>
-        <v>253305.70212687034</v>
+        <v>223343.30520163168</v>
       </c>
       <c r="G11" s="113">
         <f t="shared" si="4"/>
-        <v>253305.70212687031</v>
+        <v>223343.30520163165</v>
       </c>
       <c r="H11" s="120">
         <f t="shared" si="4"/>
-        <v>253305.70212687031</v>
+        <v>223343.30520163165</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -9654,23 +9654,23 @@
       <c r="C12" s="121"/>
       <c r="D12" s="122">
         <f>SUM(D7:D11)</f>
-        <v>5994901.617002598</v>
+        <v>9678209.8920707069</v>
       </c>
       <c r="E12" s="122">
         <f t="shared" ref="E12:H12" si="5">SUM(E7:E11)</f>
-        <v>5994901.617002598</v>
+        <v>8003135.1030584695</v>
       </c>
       <c r="F12" s="122">
         <f t="shared" si="5"/>
-        <v>5994901.617002598</v>
+        <v>5630112.4852911327</v>
       </c>
       <c r="G12" s="122">
         <f t="shared" si="5"/>
-        <v>4306196.9361567963</v>
+        <v>3943405.2324663098</v>
       </c>
       <c r="H12" s="123">
         <f t="shared" si="5"/>
-        <v>4306196.9361567963</v>
+        <v>3236733.055851772</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -9682,7 +9682,7 @@
       </c>
       <c r="D14" s="95">
         <f>_Constructions_Select*_PIBPNB_Select</f>
-        <v>20264456.170149628</v>
+        <v>17867464.416130535</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -9748,23 +9748,23 @@
       <c r="C19" s="102"/>
       <c r="D19" s="103">
         <f>D14</f>
-        <v>20264456.170149628</v>
+        <v>17867464.416130535</v>
       </c>
       <c r="E19" s="104">
         <f>D19-D22</f>
-        <v>19251233.361642148</v>
+        <v>16974091.195324007</v>
       </c>
       <c r="F19" s="104">
         <f t="shared" ref="F19:H19" si="7">E19-E22</f>
-        <v>18238010.553134669</v>
+        <v>16080717.974517481</v>
       </c>
       <c r="G19" s="104">
         <f t="shared" si="7"/>
-        <v>17224787.744627185</v>
+        <v>15187344.753710955</v>
       </c>
       <c r="H19" s="105">
         <f t="shared" si="7"/>
-        <v>16211564.936119704</v>
+        <v>14293971.532904429</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -9835,23 +9835,23 @@
       <c r="C22" s="109"/>
       <c r="D22" s="110">
         <f>D19*D21</f>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652684</v>
       </c>
       <c r="E22" s="110">
         <f t="shared" ref="E22:H22" si="9">E19*E21</f>
-        <v>1013222.8085074815</v>
+        <v>893373.2208065266</v>
       </c>
       <c r="F22" s="110">
         <f t="shared" si="9"/>
-        <v>1013222.8085074816</v>
+        <v>893373.22080652672</v>
       </c>
       <c r="G22" s="110">
         <f t="shared" si="9"/>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652672</v>
       </c>
       <c r="H22" s="111">
         <f t="shared" si="9"/>
-        <v>1013222.8085074815</v>
+        <v>893373.22080652684</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="D24" s="95">
         <f>_Equipement_Select*_PIBPNB_Select</f>
-        <v>30396684.25522444</v>
+        <v>26801196.624195807</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -9887,7 +9887,7 @@
       </c>
       <c r="D26" s="94">
         <f>_Equipement_CoefDegressif_Select</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -9929,23 +9929,23 @@
       <c r="C29" s="102"/>
       <c r="D29" s="103">
         <f>D24</f>
-        <v>30396684.25522444</v>
+        <v>26801196.624195807</v>
       </c>
       <c r="E29" s="104">
         <f>D29-D32</f>
-        <v>27357015.829701997</v>
+        <v>20100897.468146853</v>
       </c>
       <c r="F29" s="104">
         <f t="shared" ref="F29" si="13">E29-E32</f>
-        <v>24317347.404179554</v>
+        <v>15075673.10111014</v>
       </c>
       <c r="G29" s="104">
         <f t="shared" ref="G29" si="14">F29-F32</f>
-        <v>21277678.978657112</v>
+        <v>11306754.825832605</v>
       </c>
       <c r="H29" s="105">
         <f t="shared" ref="H29" si="15">G29-G32</f>
-        <v>18238010.553134669</v>
+        <v>8480066.119374454</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -9987,23 +9987,23 @@
       <c r="C31" s="102"/>
       <c r="D31" s="106">
         <f>IF(D28=0,0,IF($D26*$D30&gt;100%,100%,IF($D26*$D30&gt;D30,$D26*$D30,D30)))</f>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E31" s="106">
         <f>IF(E28=0,0,IF($D26*$D30&gt;100%,100%,IF($D26*$D30&gt;E30,$D26*$D30,E30)))</f>
-        <v>0.1111111111111111</v>
+        <v>0.25</v>
       </c>
       <c r="F31" s="106">
         <f>IF(F28=0,0,IF($D26*$D30&gt;100%,100%,IF($D26*$D30&gt;F30,$D26*$D30,F30)))</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="G31" s="106">
         <f>IF(G28=0,0,IF($D26*$D30&gt;100%,100%,IF($D26*$D30&gt;G30,$D26*$D30,G30)))</f>
-        <v>0.14285714285714285</v>
+        <v>0.25</v>
       </c>
       <c r="H31" s="107">
         <f>IF(H28=0,0,IF($D26*$D30&gt;100%,100%,IF($D26*$D30&gt;H30,$D26*$D30,H30)))</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -10016,23 +10016,23 @@
       <c r="C32" s="109"/>
       <c r="D32" s="110">
         <f>D29*D31</f>
-        <v>3039668.4255224443</v>
+        <v>6700299.1560489517</v>
       </c>
       <c r="E32" s="110">
         <f t="shared" ref="E32:H32" si="17">E29*E31</f>
-        <v>3039668.4255224438</v>
+        <v>5025224.3670367133</v>
       </c>
       <c r="F32" s="110">
         <f t="shared" si="17"/>
-        <v>3039668.4255224443</v>
+        <v>3768918.275277535</v>
       </c>
       <c r="G32" s="110">
         <f t="shared" si="17"/>
-        <v>3039668.4255224443</v>
+        <v>2826688.7064581513</v>
       </c>
       <c r="H32" s="111">
         <f t="shared" si="17"/>
-        <v>3039668.4255224448</v>
+        <v>2120016.5298436135</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -10044,7 +10044,7 @@
       </c>
       <c r="D34" s="95">
         <f>_Camion_Select*_PIBPNB_Select</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -10110,15 +10110,15 @@
       <c r="C39" s="102"/>
       <c r="D39" s="103">
         <f>D34</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
       <c r="E39" s="104">
         <f>D39-D42</f>
-        <v>1688704.6808458024</v>
+        <v>1488955.3680108781</v>
       </c>
       <c r="F39" s="104">
         <f t="shared" ref="F39" si="21">E39-E42</f>
-        <v>844352.34042290121</v>
+        <v>744477.68400543905</v>
       </c>
       <c r="G39" s="104">
         <f t="shared" ref="G39" si="22">F39-F42</f>
@@ -10197,15 +10197,15 @@
       <c r="C42" s="109"/>
       <c r="D42" s="110">
         <f>D39*D41</f>
-        <v>844352.34042290109</v>
+        <v>744477.68400543893</v>
       </c>
       <c r="E42" s="110">
         <f t="shared" ref="E42:H42" si="25">E39*E41</f>
-        <v>844352.34042290121</v>
+        <v>744477.68400543905</v>
       </c>
       <c r="F42" s="110">
         <f t="shared" si="25"/>
-        <v>844352.34042290121</v>
+        <v>744477.68400543905</v>
       </c>
       <c r="G42" s="110">
         <f t="shared" si="25"/>
@@ -10225,7 +10225,7 @@
       </c>
       <c r="D44" s="95">
         <f>_Informatique_Select*_PIBPNB_Select</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -10237,7 +10237,7 @@
       </c>
       <c r="D45" s="94">
         <f>_Informatique_DureeLineaire_Select</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -10262,15 +10262,15 @@
       <c r="C48" s="97"/>
       <c r="D48" s="98">
         <f>D45</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48" s="99">
         <f>IF(D48-1&gt;0,D48-1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" s="99">
         <f t="shared" ref="F48" si="26">IF(E48-1&gt;0,E48-1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="99">
         <f t="shared" ref="G48" si="27">IF(F48-1&gt;0,F48-1,0)</f>
@@ -10291,15 +10291,15 @@
       <c r="C49" s="102"/>
       <c r="D49" s="103">
         <f>D44</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
       <c r="E49" s="104">
         <f>D49-D52</f>
-        <v>1688704.6808458024</v>
+        <v>1116716.5260081585</v>
       </c>
       <c r="F49" s="104">
         <f t="shared" ref="F49" si="29">E49-E52</f>
-        <v>844352.34042290121</v>
+        <v>0</v>
       </c>
       <c r="G49" s="104">
         <f t="shared" ref="G49" si="30">F49-F52</f>
@@ -10320,15 +10320,15 @@
       <c r="C50" s="102"/>
       <c r="D50" s="106">
         <f>IF(D48&gt;0,1/D48,0)</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="E50" s="106">
         <f t="shared" ref="E50:H50" si="32">IF(E48&gt;0,1/E48,0)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F50" s="106">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="106">
         <f t="shared" si="32"/>
@@ -10349,15 +10349,15 @@
       <c r="C51" s="102"/>
       <c r="D51" s="106">
         <f>IF(D48=0,0,IF($D46*$D50&gt;100%,100%,IF($D46*$D50&gt;D50,$D46*$D50,D50)))</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="E51" s="106">
         <f>IF(E48=0,0,IF($D46*$D50&gt;100%,100%,IF($D46*$D50&gt;E50,$D46*$D50,E50)))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F51" s="106">
         <f>IF(F48=0,0,IF($D46*$D50&gt;100%,100%,IF($D46*$D50&gt;F50,$D46*$D50,F50)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="106">
         <f>IF(G48=0,0,IF($D46*$D50&gt;100%,100%,IF($D46*$D50&gt;G50,$D46*$D50,G50)))</f>
@@ -10378,15 +10378,15 @@
       <c r="C52" s="109"/>
       <c r="D52" s="110">
         <f>D49*D51</f>
-        <v>844352.34042290109</v>
+        <v>1116716.5260081585</v>
       </c>
       <c r="E52" s="110">
         <f t="shared" ref="E52:H52" si="33">E49*E51</f>
-        <v>844352.34042290121</v>
+        <v>1116716.5260081585</v>
       </c>
       <c r="F52" s="110">
         <f t="shared" si="33"/>
-        <v>844352.34042290121</v>
+        <v>0</v>
       </c>
       <c r="G52" s="110">
         <f t="shared" si="33"/>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="D54" s="95">
         <f>_Bureau_Select*_PIBPNB_Select</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -10472,23 +10472,23 @@
       <c r="C59" s="102"/>
       <c r="D59" s="103">
         <f>D54</f>
-        <v>2533057.0212687035</v>
+        <v>2233433.0520163169</v>
       </c>
       <c r="E59" s="104">
         <f>D59-D62</f>
-        <v>2279751.3191418331</v>
+        <v>2010089.7468146852</v>
       </c>
       <c r="F59" s="104">
         <f t="shared" ref="F59" si="37">E59-E62</f>
-        <v>2026445.6170149627</v>
+        <v>1786746.4416130534</v>
       </c>
       <c r="G59" s="104">
         <f t="shared" ref="G59" si="38">F59-F62</f>
-        <v>1773139.9148880923</v>
+        <v>1563403.1364114217</v>
       </c>
       <c r="H59" s="105">
         <f t="shared" ref="H59" si="39">G59-G62</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.83120979</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -10559,23 +10559,23 @@
       <c r="C62" s="109"/>
       <c r="D62" s="110">
         <f>D59*D61</f>
-        <v>253305.70212687037</v>
+        <v>223343.30520163171</v>
       </c>
       <c r="E62" s="110">
         <f t="shared" ref="E62:H62" si="41">E59*E61</f>
-        <v>253305.70212687034</v>
+        <v>223343.30520163168</v>
       </c>
       <c r="F62" s="110">
         <f t="shared" si="41"/>
-        <v>253305.70212687034</v>
+        <v>223343.30520163168</v>
       </c>
       <c r="G62" s="110">
         <f t="shared" si="41"/>
-        <v>253305.70212687031</v>
+        <v>223343.30520163165</v>
       </c>
       <c r="H62" s="111">
         <f t="shared" si="41"/>
-        <v>253305.70212687031</v>
+        <v>223343.30520163165</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -10592,7 +10592,7 @@
       </c>
       <c r="D65" s="95">
         <f>(_Terrain_Select+_Constructions_Select+_Equipement_Select+_Camion_Select+_Informatique_Select+_Bureau_Select)*_PIBPNB_Select</f>
-        <v>73458653.616792396</v>
+        <v>64769558.508473195</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -10825,23 +10825,23 @@
       <c r="C80" s="116"/>
       <c r="D80" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="E80" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="F80" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="G80" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="H80" s="128">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -10854,23 +10854,23 @@
       <c r="C81" s="119"/>
       <c r="D81" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="E81" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="F81" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="G81" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="H81" s="130">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -10883,23 +10883,23 @@
       <c r="C82" s="119"/>
       <c r="D82" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="E82" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="F82" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="G82" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="H82" s="130">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -10912,23 +10912,23 @@
       <c r="C83" s="119"/>
       <c r="D83" s="114">
         <f>SUM(D80:D82)</f>
-        <v>33942964.085000619</v>
+        <v>29928002.897018649</v>
       </c>
       <c r="E83" s="114">
         <f t="shared" ref="E83:H83" si="47">SUM(E80:E82)</f>
-        <v>33942964.085000619</v>
+        <v>29928002.897018649</v>
       </c>
       <c r="F83" s="114">
         <f t="shared" si="47"/>
-        <v>33942964.085000619</v>
+        <v>29928002.897018649</v>
       </c>
       <c r="G83" s="114">
         <f t="shared" si="47"/>
-        <v>33942964.085000619</v>
+        <v>29928002.897018649</v>
       </c>
       <c r="H83" s="131">
         <f t="shared" si="47"/>
-        <v>33942964.085000619</v>
+        <v>29928002.897018649</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -10941,23 +10941,23 @@
       <c r="C84" s="119"/>
       <c r="D84" s="125">
         <f>_CFE_Taux_Select1</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E84" s="125">
         <f>_CFE_Taux_Select2</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F84" s="125">
         <f>_CFE_Taux_Select3</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="G84" s="125">
         <f>_CFE_Taux_Select4</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H84" s="126">
         <f>_CFE_Taux_Select5</f>
-        <v>8.6999999999999994E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -10970,23 +10970,23 @@
       <c r="C85" s="121"/>
       <c r="D85" s="110">
         <f>D83*D84</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="E85" s="110">
         <f t="shared" ref="E85:H85" si="48">E83*E84</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="F85" s="110">
         <f t="shared" si="48"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="G85" s="110">
         <f t="shared" si="48"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="H85" s="111">
         <f t="shared" si="48"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -11004,23 +11004,23 @@
       <c r="C88" s="116"/>
       <c r="D88" s="127">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="E88" s="127">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="F88" s="127">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="G88" s="127">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="H88" s="128">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -11033,23 +11033,23 @@
       <c r="C89" s="119"/>
       <c r="D89" s="125">
         <f>_IRC_Taux_Select1</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E89" s="125">
         <f>_IRC_Taux_Select2</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F89" s="125">
         <f>_IRC_Taux_Select3</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="G89" s="125">
         <f>_IRC_Taux_Select4</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="H89" s="126">
         <f>_IRC_Taux_Select5</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -11062,23 +11062,23 @@
       <c r="C90" s="121"/>
       <c r="D90" s="110">
         <f>D88*D89</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="E90" s="110">
         <f t="shared" ref="E90" si="49">E88*E89</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="F90" s="110">
         <f t="shared" ref="F90" si="50">F88*F89</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="G90" s="110">
         <f t="shared" ref="G90" si="51">G88*G89</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="H90" s="111">
         <f t="shared" ref="H90" si="52">H88*H89</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -11096,23 +11096,23 @@
       <c r="C93" s="91"/>
       <c r="D93" s="93">
         <f>_Ventes_Select*_PIBPNB_Select</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="E93" s="93">
         <f>_Ventes_Select*_PIBPNB_Select</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="F93" s="93">
         <f>_Ventes_Select*_PIBPNB_Select</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="G93" s="93">
         <f>_Ventes_Select*_PIBPNB_Select</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="H93" s="137">
         <f>_Ventes_Select*_PIBPNB_Select</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -11125,23 +11125,23 @@
       <c r="C94" s="119"/>
       <c r="D94" s="129">
         <f>_Achats_Select*_PIBPNB_Select</f>
-        <v>443284978.72202307</v>
+        <v>390850784.1028555</v>
       </c>
       <c r="E94" s="129">
         <f>_Achats_Select*_PIBPNB_Select</f>
-        <v>443284978.72202307</v>
+        <v>390850784.1028555</v>
       </c>
       <c r="F94" s="129">
         <f>_Achats_Select*_PIBPNB_Select</f>
-        <v>443284978.72202307</v>
+        <v>390850784.1028555</v>
       </c>
       <c r="G94" s="129">
         <f>_Achats_Select*_PIBPNB_Select</f>
-        <v>443284978.72202307</v>
+        <v>390850784.1028555</v>
       </c>
       <c r="H94" s="130">
         <f>_Achats_Select*_PIBPNB_Select</f>
-        <v>443284978.72202307</v>
+        <v>390850784.1028555</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -11212,23 +11212,23 @@
       <c r="C97" s="119"/>
       <c r="D97" s="129">
         <f>_DepensesAdministratives_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="E97" s="129">
         <f>_DepensesAdministratives_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="F97" s="129">
         <f>_DepensesAdministratives_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="G97" s="129">
         <f>_DepensesAdministratives_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="H97" s="130">
         <f>_DepensesAdministratives_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -11241,23 +11241,23 @@
       <c r="C98" s="119"/>
       <c r="D98" s="129">
         <f>_DepensesPublicitaires_Select*_PIBPNB_Select</f>
-        <v>5319419.744664277</v>
+        <v>4690209.4092342658</v>
       </c>
       <c r="E98" s="129">
         <f>_DepensesPublicitaires_Select*_PIBPNB_Select</f>
-        <v>5319419.744664277</v>
+        <v>4690209.4092342658</v>
       </c>
       <c r="F98" s="129">
         <f>_DepensesPublicitaires_Select*_PIBPNB_Select</f>
-        <v>5319419.744664277</v>
+        <v>4690209.4092342658</v>
       </c>
       <c r="G98" s="129">
         <f>_DepensesPublicitaires_Select*_PIBPNB_Select</f>
-        <v>5319419.744664277</v>
+        <v>4690209.4092342658</v>
       </c>
       <c r="H98" s="130">
         <f>_DepensesPublicitaires_Select*_PIBPNB_Select</f>
-        <v>5319419.744664277</v>
+        <v>4690209.4092342658</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -11270,23 +11270,23 @@
       <c r="C99" s="119"/>
       <c r="D99" s="129">
         <f>_DepensesDEntretien_Select*_PIBPNB_Select</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.8312097902</v>
       </c>
       <c r="E99" s="129">
         <f>_DepensesDEntretien_Select*_PIBPNB_Select</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.8312097902</v>
       </c>
       <c r="F99" s="129">
         <f>_DepensesDEntretien_Select*_PIBPNB_Select</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.8312097902</v>
       </c>
       <c r="G99" s="129">
         <f>_DepensesDEntretien_Select*_PIBPNB_Select</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.8312097902</v>
       </c>
       <c r="H99" s="130">
         <f>_DepensesDEntretien_Select*_PIBPNB_Select</f>
-        <v>1519834.2127612219</v>
+        <v>1340059.8312097902</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -11299,23 +11299,23 @@
       <c r="C100" s="116"/>
       <c r="D100" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="E100" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="F100" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="G100" s="127">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
       <c r="H100" s="128">
         <f>_Nombre_Cadres_Select*_Indice_Cadres_Select*_PIBPNB_Select</f>
-        <v>4559502.6382836662</v>
+        <v>4020179.4936293708</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -11328,23 +11328,23 @@
       <c r="C101" s="119"/>
       <c r="D101" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="E101" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="F101" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="G101" s="129">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
       <c r="H101" s="130">
         <f>_Nombre_Secretaires_Select*_Indice_Secretaires_Select*_PIBPNB_Select</f>
-        <v>5066114.042537407</v>
+        <v>4466866.1040326338</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -11357,23 +11357,23 @@
       <c r="C102" s="119"/>
       <c r="D102" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="E102" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="F102" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="G102" s="129">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
       <c r="H102" s="130">
         <f>_Nombre_Ouvriers_Select*_Indice_Ouvriers_Select*_PIBPNB_Select</f>
-        <v>24317347.404179551</v>
+        <v>21440957.299356643</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -11386,23 +11386,23 @@
       <c r="C103" s="121"/>
       <c r="D103" s="135">
         <f>D$85</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="E103" s="135">
         <f t="shared" ref="E103:H103" si="54">E$85</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="F103" s="135">
         <f t="shared" si="54"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="G103" s="135">
         <f t="shared" si="54"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="H103" s="136">
         <f t="shared" si="54"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -11415,23 +11415,23 @@
       <c r="C104" s="119"/>
       <c r="D104" s="129">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="E104" s="129">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="F104" s="129">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="G104" s="129">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
       <c r="H104" s="130">
         <f>_ChargesFinancieres_Select*_PIBPNB_Select</f>
-        <v>2786362.7233955739</v>
+        <v>2456776.3572179489</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -11444,23 +11444,23 @@
       <c r="C105" s="91"/>
       <c r="D105" s="112">
         <f>D$12</f>
-        <v>5994901.617002598</v>
+        <v>9678209.8920707069</v>
       </c>
       <c r="E105" s="112">
         <f t="shared" ref="E105:H105" si="55">E$12</f>
-        <v>5994901.617002598</v>
+        <v>8003135.1030584695</v>
       </c>
       <c r="F105" s="112">
         <f t="shared" si="55"/>
-        <v>5994901.617002598</v>
+        <v>5630112.4852911327</v>
       </c>
       <c r="G105" s="112">
         <f t="shared" si="55"/>
-        <v>4306196.9361567963</v>
+        <v>3943405.2324663098</v>
       </c>
       <c r="H105" s="134">
         <f t="shared" si="55"/>
-        <v>4306196.9361567963</v>
+        <v>3236733.055851772</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -11473,23 +11473,23 @@
       <c r="C106" s="116"/>
       <c r="D106" s="153">
         <f>D93-SUM(D94:D105)</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E106" s="153">
         <f>E93-SUM(E94:E105)</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F106" s="153">
         <f>F93-SUM(F94:F105)</f>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G106" s="153">
         <f>G93-SUM(G94:G105)</f>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H106" s="154">
         <f>H93-SUM(H94:H105)</f>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -11502,23 +11502,23 @@
       <c r="C107" s="121"/>
       <c r="D107" s="132">
         <f>D106/D$93</f>
-        <v>5.8416825396825398E-2</v>
+        <v>5.2050793650793507E-2</v>
       </c>
       <c r="E107" s="132">
         <f t="shared" ref="E107:H107" si="56">E106/E$93</f>
-        <v>5.8416825396825398E-2</v>
+        <v>5.5622222222222115E-2</v>
       </c>
       <c r="F107" s="132">
         <f t="shared" si="56"/>
-        <v>5.8416825396825398E-2</v>
+        <v>6.0681746031745913E-2</v>
       </c>
       <c r="G107" s="132">
         <f t="shared" si="56"/>
-        <v>6.1591428571428568E-2</v>
+        <v>6.4277976190476122E-2</v>
       </c>
       <c r="H107" s="133">
         <f t="shared" si="56"/>
-        <v>6.1591428571428568E-2</v>
+        <v>6.578467261904751E-2</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -11536,23 +11536,23 @@
       <c r="C110" s="116"/>
       <c r="D110" s="117">
         <f>D106</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E110" s="117">
         <f t="shared" ref="E110:H110" si="57">E106</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F110" s="117">
         <f t="shared" si="57"/>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G110" s="117">
         <f t="shared" si="57"/>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H110" s="118">
         <f t="shared" si="57"/>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -11594,23 +11594,23 @@
       <c r="C112" s="121"/>
       <c r="D112" s="122">
         <f>D110-D111</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E112" s="122">
         <f t="shared" ref="E112:H112" si="58">E110-E111</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F112" s="122">
         <f t="shared" si="58"/>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G112" s="122">
         <f t="shared" si="58"/>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H112" s="123">
         <f t="shared" si="58"/>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -11628,23 +11628,23 @@
       <c r="C115" s="116"/>
       <c r="D115" s="117">
         <f>D$112</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E115" s="117">
         <f t="shared" ref="E115:H115" si="59">E$112</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F115" s="117">
         <f t="shared" si="59"/>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G115" s="117">
         <f t="shared" si="59"/>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H115" s="118">
         <f t="shared" si="59"/>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -11657,23 +11657,23 @@
       <c r="C116" s="119"/>
       <c r="D116" s="125">
         <f>_IS_Taux_Select1</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E116" s="125">
         <f>_IS_Taux_Select2</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F116" s="125">
         <f>_IS_Taux_Select3</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="G116" s="125">
         <f>_IS_Taux_Select4</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="H116" s="126">
         <f>_IS_Taux_Select5</f>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -11686,23 +11686,23 @@
       <c r="C117" s="121"/>
       <c r="D117" s="110">
         <f>D115*D116</f>
-        <v>10876026.505276751</v>
+        <v>7323873.6641718866</v>
       </c>
       <c r="E117" s="110">
         <f t="shared" ref="E117:H117" si="60">E115*E116</f>
-        <v>10876026.505276751</v>
+        <v>7826396.1008755621</v>
       </c>
       <c r="F117" s="110">
         <f t="shared" si="60"/>
-        <v>10876026.505276751</v>
+        <v>8538302.8862057626</v>
       </c>
       <c r="G117" s="110">
         <f t="shared" si="60"/>
-        <v>11467073.143572779</v>
+        <v>9044315.0620532148</v>
       </c>
       <c r="H117" s="111">
         <f t="shared" si="60"/>
-        <v>11467073.143572779</v>
+        <v>9256316.7150375713</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -11720,23 +11720,23 @@
       <c r="C120" s="116"/>
       <c r="D120" s="117">
         <f>D$93</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="E120" s="117">
         <f t="shared" ref="E120:H120" si="61">E$93</f>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="F120" s="117">
         <f t="shared" si="61"/>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="G120" s="117">
         <f t="shared" si="61"/>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
       <c r="H120" s="118">
         <f t="shared" si="61"/>
-        <v>531941974.46642768</v>
+        <v>469020940.92342657</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -11749,23 +11749,23 @@
       <c r="C121" s="119"/>
       <c r="D121" s="125">
         <f>_IMF_Taux_Select1</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E121" s="125">
         <f>_IMF_Taux_Select2</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F121" s="125">
         <f>_IMF_Taux_Select3</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="G121" s="125">
         <f>_IMF_Taux_Select4</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="H121" s="126">
         <f>_IMF_Taux_Select5</f>
-        <v>1.4999999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -11778,23 +11778,23 @@
       <c r="C122" s="121"/>
       <c r="D122" s="110">
         <f>D120*D121</f>
-        <v>7979129.616996415</v>
+        <v>3517657.0569256991</v>
       </c>
       <c r="E122" s="110">
         <f t="shared" ref="E122" si="62">E120*E121</f>
-        <v>7979129.616996415</v>
+        <v>3517657.0569256991</v>
       </c>
       <c r="F122" s="110">
         <f t="shared" ref="F122" si="63">F120*F121</f>
-        <v>7979129.616996415</v>
+        <v>3517657.0569256991</v>
       </c>
       <c r="G122" s="110">
         <f t="shared" ref="G122" si="64">G120*G121</f>
-        <v>7979129.616996415</v>
+        <v>3517657.0569256991</v>
       </c>
       <c r="H122" s="111">
         <f t="shared" ref="H122" si="65">H120*H121</f>
-        <v>7979129.616996415</v>
+        <v>3517657.0569256991</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -11810,23 +11810,23 @@
       <c r="C125" s="116"/>
       <c r="D125" s="155">
         <f>IF(D$117&gt;D$122,D$117,D$122)</f>
-        <v>10876026.505276751</v>
+        <v>7323873.6641718866</v>
       </c>
       <c r="E125" s="155">
         <f>IF(E$117&gt;E$122,E$117,E$122)</f>
-        <v>10876026.505276751</v>
+        <v>7826396.1008755621</v>
       </c>
       <c r="F125" s="155">
         <f>IF(F$117&gt;F$122,F$117,F$122)</f>
-        <v>10876026.505276751</v>
+        <v>8538302.8862057626</v>
       </c>
       <c r="G125" s="155">
         <f>IF(G$117&gt;G$122,G$117,G$122)</f>
-        <v>11467073.143572779</v>
+        <v>9044315.0620532148</v>
       </c>
       <c r="H125" s="156">
         <f>IF(H$117&gt;H$122,H$117,H$122)</f>
-        <v>11467073.143572779</v>
+        <v>9256316.7150375713</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -11839,23 +11839,23 @@
       <c r="C126" s="119"/>
       <c r="D126" s="113">
         <f>D$106</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E126" s="113">
         <f t="shared" ref="E126:H126" si="66">E$106</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F126" s="113">
         <f t="shared" si="66"/>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G126" s="113">
         <f t="shared" si="66"/>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H126" s="120">
         <f t="shared" si="66"/>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -11868,23 +11868,23 @@
       <c r="C127" s="121"/>
       <c r="D127" s="132">
         <f>D126/D$93</f>
-        <v>5.8416825396825398E-2</v>
+        <v>5.2050793650793507E-2</v>
       </c>
       <c r="E127" s="132">
         <f t="shared" ref="E127:H127" si="67">E126/E$93</f>
-        <v>5.8416825396825398E-2</v>
+        <v>5.5622222222222115E-2</v>
       </c>
       <c r="F127" s="132">
         <f t="shared" si="67"/>
-        <v>5.8416825396825398E-2</v>
+        <v>6.0681746031745913E-2</v>
       </c>
       <c r="G127" s="132">
         <f t="shared" si="67"/>
-        <v>6.1591428571428568E-2</v>
+        <v>6.4277976190476122E-2</v>
       </c>
       <c r="H127" s="133">
         <f t="shared" si="67"/>
-        <v>6.1591428571428568E-2</v>
+        <v>6.578467261904751E-2</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -11902,23 +11902,23 @@
       <c r="C130" s="116"/>
       <c r="D130" s="117">
         <f>D126</f>
-        <v>31074361.443647861</v>
+        <v>24412912.213906288</v>
       </c>
       <c r="E130" s="117">
         <f t="shared" ref="E130:H130" si="68">E126</f>
-        <v>31074361.443647861</v>
+        <v>26087987.002918541</v>
       </c>
       <c r="F130" s="117">
         <f t="shared" si="68"/>
-        <v>31074361.443647861</v>
+        <v>28461009.620685875</v>
       </c>
       <c r="G130" s="117">
         <f t="shared" si="68"/>
-        <v>32763066.124493659</v>
+        <v>30147716.873510718</v>
       </c>
       <c r="H130" s="118">
         <f t="shared" si="68"/>
-        <v>32763066.124493659</v>
+        <v>30854389.050125241</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -11960,23 +11960,23 @@
       <c r="C132" s="119"/>
       <c r="D132" s="125">
         <f>_IRVM_Taux_Select1</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E132" s="125">
         <f>_IRVM_Taux_Select2</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F132" s="125">
         <f>_IRVM_Taux_Select3</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G132" s="125">
         <f>_IRVM_Taux_Select4</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H132" s="126">
         <f>_IRVM_Taux_Select5</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -11989,23 +11989,23 @@
       <c r="C133" s="121"/>
       <c r="D133" s="110">
         <f>D130*D131*D132</f>
-        <v>3107436.1443647863</v>
+        <v>1220645.6106953144</v>
       </c>
       <c r="E133" s="110">
         <f t="shared" ref="E133:H133" si="69">E130*E131*E132</f>
-        <v>3107436.1443647863</v>
+        <v>1304399.3501459272</v>
       </c>
       <c r="F133" s="110">
         <f t="shared" si="69"/>
-        <v>3107436.1443647863</v>
+        <v>1423050.4810342938</v>
       </c>
       <c r="G133" s="110">
         <f t="shared" si="69"/>
-        <v>3276306.6124493661</v>
+        <v>1507385.8436755361</v>
       </c>
       <c r="H133" s="111">
         <f t="shared" si="69"/>
-        <v>3276306.6124493661</v>
+        <v>1542719.4525062621</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -12063,27 +12063,27 @@
       <c r="C140" s="116"/>
       <c r="D140" s="117">
         <f>D$85</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="E140" s="117">
         <f t="shared" ref="E140:H140" si="70">E$85</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="F140" s="117">
         <f t="shared" si="70"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="G140" s="117">
         <f t="shared" si="70"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="H140" s="117">
         <f t="shared" si="70"/>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="I140" s="162">
         <f t="shared" ref="I140:I145" si="71">NPV(_TauxDActualisation_Select,D140:H140)</f>
-        <v>11790623.964961573</v>
+        <v>4779753.502265133</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -12096,27 +12096,27 @@
       <c r="C141" s="119"/>
       <c r="D141" s="113">
         <f>D125</f>
-        <v>10876026.505276751</v>
+        <v>7323873.6641718866</v>
       </c>
       <c r="E141" s="113">
         <f>E125</f>
-        <v>10876026.505276751</v>
+        <v>7826396.1008755621</v>
       </c>
       <c r="F141" s="113">
         <f>F125</f>
-        <v>10876026.505276751</v>
+        <v>8538302.8862057626</v>
       </c>
       <c r="G141" s="113">
         <f>G125</f>
-        <v>11467073.143572779</v>
+        <v>9044315.0620532148</v>
       </c>
       <c r="H141" s="113">
         <f>H125</f>
-        <v>11467073.143572779</v>
+        <v>9256316.7150375713</v>
       </c>
       <c r="I141" s="163">
         <f t="shared" si="71"/>
-        <v>44261513.525375903</v>
+        <v>33216753.010250647</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -12129,27 +12129,27 @@
       <c r="C142" s="119"/>
       <c r="D142" s="113">
         <f>D$133</f>
-        <v>3107436.1443647863</v>
+        <v>1220645.6106953144</v>
       </c>
       <c r="E142" s="113">
         <f>E$133</f>
-        <v>3107436.1443647863</v>
+        <v>1304399.3501459272</v>
       </c>
       <c r="F142" s="113">
         <f t="shared" ref="F142:H142" si="72">F$133</f>
-        <v>3107436.1443647863</v>
+        <v>1423050.4810342938</v>
       </c>
       <c r="G142" s="113">
         <f t="shared" si="72"/>
-        <v>3276306.6124493661</v>
+        <v>1507385.8436755361</v>
       </c>
       <c r="H142" s="113">
         <f t="shared" si="72"/>
-        <v>3276306.6124493661</v>
+        <v>1542719.4525062621</v>
       </c>
       <c r="I142" s="163">
         <f t="shared" si="71"/>
-        <v>12646146.721535973</v>
+        <v>5536125.5017084414</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -12162,27 +12162,27 @@
       <c r="C143" s="119"/>
       <c r="D143" s="113">
         <f>D$90</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="E143" s="113">
         <f t="shared" ref="E143:H143" si="73">E$90</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="F143" s="113">
         <f t="shared" si="73"/>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="G143" s="113">
         <f t="shared" si="73"/>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="H143" s="113">
         <f t="shared" si="73"/>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="I143" s="163">
         <f t="shared" si="71"/>
-        <v>2225027.6825283477</v>
+        <v>1471379.3430480356</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -12228,27 +12228,27 @@
       <c r="C145" s="121"/>
       <c r="D145" s="122">
         <f>SUM(D140:D144)</f>
-        <v>17493773.069715708</v>
+        <v>10110155.844330639</v>
       </c>
       <c r="E145" s="122">
         <f>SUM(E140:E144)</f>
-        <v>17493773.069715708</v>
+        <v>10696432.020484928</v>
       </c>
       <c r="F145" s="122">
         <f>SUM(F140:F144)</f>
-        <v>17493773.069715708</v>
+        <v>11526989.936703496</v>
       </c>
       <c r="G145" s="122">
         <f>SUM(G140:G144)</f>
-        <v>18253690.176096316</v>
+        <v>12117337.475192189</v>
       </c>
       <c r="H145" s="122">
         <f>SUM(H140:H144)</f>
-        <v>18253690.176096316</v>
+        <v>12364672.737007273</v>
       </c>
       <c r="I145" s="165">
         <f t="shared" si="71"/>
-        <v>70923311.894401804</v>
+        <v>45004011.35727226</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -12269,27 +12269,27 @@
       <c r="C147" s="116"/>
       <c r="D147" s="117">
         <f t="shared" ref="D147:H148" si="75">D140*D$136</f>
-        <v>2953037.8753950535</v>
+        <v>1197120.1158807459</v>
       </c>
       <c r="E147" s="117">
         <f t="shared" si="75"/>
-        <v>2734294.3290694938</v>
+        <v>1108444.5517414312</v>
       </c>
       <c r="F147" s="117">
         <f t="shared" si="75"/>
-        <v>2531754.0083976793</v>
+        <v>1026337.5479087328</v>
       </c>
       <c r="G147" s="117">
         <f t="shared" si="75"/>
-        <v>2344216.6744422955</v>
+        <v>950312.54435993766</v>
       </c>
       <c r="H147" s="117">
         <f t="shared" si="75"/>
-        <v>2170570.9948539771</v>
+        <v>879919.02255549782</v>
       </c>
       <c r="I147" s="162">
         <f>SUM(D147:H147)</f>
-        <v>12733873.882158499</v>
+        <v>5162133.7824463444</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -12302,27 +12302,27 @@
       <c r="C148" s="119"/>
       <c r="D148" s="113">
         <f t="shared" si="75"/>
-        <v>10876026.505276751</v>
+        <v>7323873.6641718866</v>
       </c>
       <c r="E148" s="113">
         <f t="shared" si="75"/>
-        <v>10070394.912293287</v>
+        <v>7246663.0563662602</v>
       </c>
       <c r="F148" s="113">
         <f t="shared" si="75"/>
-        <v>9324439.733604895</v>
+        <v>7320218.5238389596</v>
       </c>
       <c r="G148" s="113">
         <f t="shared" si="75"/>
-        <v>9102932.3715045806</v>
+        <v>7179668.8942021774</v>
       </c>
       <c r="H148" s="113">
         <f t="shared" si="75"/>
-        <v>8428641.0847264621</v>
+        <v>6803669.1124914158</v>
       </c>
       <c r="I148" s="163">
         <f t="shared" ref="I148:I152" si="76">SUM(D148:H148)</f>
-        <v>47802434.607405975</v>
+        <v>35874093.251070701</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -12335,27 +12335,27 @@
       <c r="C149" s="119"/>
       <c r="D149" s="113">
         <f t="shared" ref="D149:H149" si="77">D142*D$136</f>
-        <v>3107436.1443647863</v>
+        <v>1220645.6106953144</v>
       </c>
       <c r="E149" s="113">
         <f>E142*E$136</f>
-        <v>2877255.6892266539</v>
+        <v>1207777.1760610435</v>
       </c>
       <c r="F149" s="113">
         <f t="shared" si="77"/>
-        <v>2664125.6381728277</v>
+        <v>1220036.4206398265</v>
       </c>
       <c r="G149" s="113">
         <f t="shared" si="77"/>
-        <v>2600837.8204298806</v>
+        <v>1196611.4823670299</v>
       </c>
       <c r="H149" s="113">
         <f t="shared" si="77"/>
-        <v>2408183.167064704</v>
+        <v>1133944.8520819028</v>
       </c>
       <c r="I149" s="163">
         <f t="shared" si="76"/>
-        <v>13657838.459258853</v>
+        <v>5979015.5418451168</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -12368,27 +12368,27 @@
       <c r="C150" s="119"/>
       <c r="D150" s="113">
         <f t="shared" ref="D150:H150" si="78">D143*D$136</f>
-        <v>557272.54467911483</v>
+        <v>368516.45358269231</v>
       </c>
       <c r="E150" s="113">
         <f t="shared" si="78"/>
-        <v>515993.09692510625</v>
+        <v>341218.93850249285</v>
       </c>
       <c r="F150" s="113">
         <f t="shared" si="78"/>
-        <v>477771.3860417651</v>
+        <v>315943.46157638228</v>
       </c>
       <c r="G150" s="113">
         <f t="shared" si="78"/>
-        <v>442380.9130016343</v>
+        <v>292540.24220035394</v>
       </c>
       <c r="H150" s="113">
         <f t="shared" si="78"/>
-        <v>409611.95648299472</v>
+        <v>270870.59462995734</v>
       </c>
       <c r="I150" s="163">
         <f t="shared" si="76"/>
-        <v>2403029.8971306151</v>
+        <v>1589089.6904918787</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -12434,27 +12434,27 @@
       <c r="C152" s="121"/>
       <c r="D152" s="122">
         <f>SUM(D147:D151)</f>
-        <v>17493773.069715708</v>
+        <v>10110155.844330639</v>
       </c>
       <c r="E152" s="122">
         <f t="shared" ref="E152" si="80">SUM(E147:E151)</f>
-        <v>16197938.02751454</v>
+        <v>9904103.7226712275</v>
       </c>
       <c r="F152" s="122">
         <f t="shared" ref="F152" si="81">SUM(F147:F151)</f>
-        <v>14998090.766217168</v>
+        <v>9882535.9539639</v>
       </c>
       <c r="G152" s="122">
         <f t="shared" ref="G152" si="82">SUM(G147:G151)</f>
-        <v>14490367.77937839</v>
+        <v>9619133.1631294992</v>
       </c>
       <c r="H152" s="122">
         <f t="shared" ref="H152" si="83">SUM(H147:H151)</f>
-        <v>13417007.203128139</v>
+        <v>9088403.5817587748</v>
       </c>
       <c r="I152" s="165">
         <f t="shared" si="76"/>
-        <v>76597176.845953941</v>
+        <v>48604332.265854038</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -12477,27 +12477,27 @@
       <c r="C156" s="116"/>
       <c r="D156" s="166">
         <f t="shared" ref="D156:I161" si="84">D140/D$171</f>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="E156" s="166">
         <f t="shared" si="84"/>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="F156" s="166">
         <f t="shared" si="84"/>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="G156" s="166">
         <f t="shared" si="84"/>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="H156" s="166">
         <f t="shared" si="84"/>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="I156" s="168">
         <f t="shared" si="84"/>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911429E-2</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -12510,27 +12510,27 @@
       <c r="C157" s="119"/>
       <c r="D157" s="167">
         <f t="shared" si="84"/>
-        <v>0.27174915611814349</v>
+        <v>0.2075443037974681</v>
       </c>
       <c r="E157" s="167">
         <f t="shared" si="84"/>
-        <v>0.27174915611814349</v>
+        <v>0.22178481012658216</v>
       </c>
       <c r="F157" s="167">
         <f t="shared" si="84"/>
-        <v>0.27174915611814349</v>
+        <v>0.24195886075949355</v>
       </c>
       <c r="G157" s="167">
         <f t="shared" si="84"/>
-        <v>0.28651708860759495</v>
+        <v>0.25629825949367097</v>
       </c>
       <c r="H157" s="167">
         <f t="shared" si="84"/>
-        <v>0.28651708860759495</v>
+        <v>0.26230597310126574</v>
       </c>
       <c r="I157" s="169">
         <f>I141/I$171</f>
-        <v>0.27698511809808679</v>
+        <v>0.23575416816926678</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -12543,27 +12543,27 @@
       <c r="C158" s="119"/>
       <c r="D158" s="167">
         <f t="shared" si="84"/>
-        <v>7.7642616033755302E-2</v>
+        <v>3.4590717299578015E-2</v>
       </c>
       <c r="E158" s="167">
         <f t="shared" si="84"/>
-        <v>7.7642616033755302E-2</v>
+        <v>3.6964135021097029E-2</v>
       </c>
       <c r="F158" s="167">
         <f t="shared" si="84"/>
-        <v>7.7642616033755302E-2</v>
+        <v>4.0326476793248925E-2</v>
       </c>
       <c r="G158" s="167">
         <f t="shared" si="84"/>
-        <v>8.1862025316455714E-2</v>
+        <v>4.2716376582278504E-2</v>
       </c>
       <c r="H158" s="167">
         <f t="shared" si="84"/>
-        <v>8.1862025316455714E-2</v>
+        <v>4.3717662183544302E-2</v>
       </c>
       <c r="I158" s="169">
         <f t="shared" si="84"/>
-        <v>7.9138605170881948E-2</v>
+        <v>3.9292361361544466E-2</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -12576,27 +12576,27 @@
       <c r="C159" s="119"/>
       <c r="D159" s="167">
         <f t="shared" si="84"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="E159" s="167">
         <f t="shared" si="84"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="F159" s="167">
         <f t="shared" si="84"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="G159" s="167">
         <f t="shared" si="84"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="H159" s="167">
         <f t="shared" si="84"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="I159" s="169">
         <f t="shared" si="84"/>
-        <v>1.3924050632911399E-2</v>
+        <v>1.0443037974683557E-2</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -12642,27 +12642,27 @@
       <c r="C161" s="121"/>
       <c r="D161" s="170">
         <f t="shared" si="84"/>
-        <v>0.43710063291139256</v>
+        <v>0.28650210970464107</v>
       </c>
       <c r="E161" s="170">
         <f t="shared" si="84"/>
-        <v>0.43710063291139256</v>
+        <v>0.30311603375527418</v>
       </c>
       <c r="F161" s="170">
         <f t="shared" si="84"/>
-        <v>0.43710063291139256</v>
+        <v>0.32665242616033752</v>
       </c>
       <c r="G161" s="170">
         <f t="shared" si="84"/>
-        <v>0.45608797468354439</v>
+        <v>0.34338172468354444</v>
       </c>
       <c r="H161" s="170">
         <f t="shared" si="84"/>
-        <v>0.45608797468354439</v>
+        <v>0.35039072389240511</v>
       </c>
       <c r="I161" s="171">
         <f t="shared" si="84"/>
-        <v>0.44383258402846248</v>
+        <v>0.31941361813840624</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
@@ -12680,27 +12680,27 @@
       <c r="C163" s="116"/>
       <c r="D163" s="166">
         <f t="shared" ref="D163:I168" si="85">D147/D$172</f>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="E163" s="166">
         <f t="shared" si="85"/>
-        <v>7.3784810126582279E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="F163" s="166">
         <f t="shared" si="85"/>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="G163" s="166">
         <f t="shared" si="85"/>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="H163" s="166">
         <f t="shared" si="85"/>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="I163" s="168">
         <f t="shared" si="85"/>
-        <v>7.3784810126582265E-2</v>
+        <v>3.3924050632911436E-2</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
@@ -12713,27 +12713,27 @@
       <c r="C164" s="119"/>
       <c r="D164" s="167">
         <f t="shared" si="85"/>
-        <v>0.27174915611814349</v>
+        <v>0.2075443037974681</v>
       </c>
       <c r="E164" s="167">
         <f t="shared" si="85"/>
-        <v>0.27174915611814354</v>
+        <v>0.22178481012658216</v>
       </c>
       <c r="F164" s="167">
         <f t="shared" si="85"/>
-        <v>0.27174915611814349</v>
+        <v>0.24195886075949358</v>
       </c>
       <c r="G164" s="167">
         <f t="shared" si="85"/>
-        <v>0.28651708860759495</v>
+        <v>0.25629825949367097</v>
       </c>
       <c r="H164" s="167">
         <f t="shared" si="85"/>
-        <v>0.28651708860759489</v>
+        <v>0.26230597310126574</v>
       </c>
       <c r="I164" s="169">
         <f t="shared" si="85"/>
-        <v>0.27698511809808679</v>
+        <v>0.23575416816926681</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -12746,27 +12746,27 @@
       <c r="C165" s="119"/>
       <c r="D165" s="167">
         <f t="shared" si="85"/>
-        <v>7.7642616033755302E-2</v>
+        <v>3.4590717299578015E-2</v>
       </c>
       <c r="E165" s="167">
         <f t="shared" si="85"/>
-        <v>7.7642616033755302E-2</v>
+        <v>3.6964135021097029E-2</v>
       </c>
       <c r="F165" s="167">
         <f t="shared" si="85"/>
-        <v>7.7642616033755288E-2</v>
+        <v>4.0326476793248925E-2</v>
       </c>
       <c r="G165" s="167">
         <f t="shared" si="85"/>
-        <v>8.1862025316455714E-2</v>
+        <v>4.2716376582278504E-2</v>
       </c>
       <c r="H165" s="167">
         <f t="shared" si="85"/>
-        <v>8.1862025316455714E-2</v>
+        <v>4.3717662183544295E-2</v>
       </c>
       <c r="I165" s="169">
         <f t="shared" si="85"/>
-        <v>7.9138605170881962E-2</v>
+        <v>3.9292361361544466E-2</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
@@ -12779,27 +12779,27 @@
       <c r="C166" s="119"/>
       <c r="D166" s="167">
         <f t="shared" si="85"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="E166" s="167">
         <f t="shared" si="85"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="F166" s="167">
         <f t="shared" si="85"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="G166" s="167">
         <f t="shared" si="85"/>
-        <v>1.3924050632911397E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="H166" s="167">
         <f t="shared" si="85"/>
-        <v>1.3924050632911399E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="I166" s="169">
         <f t="shared" si="85"/>
-        <v>1.3924050632911395E-2</v>
+        <v>1.0443037974683558E-2</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
@@ -12845,27 +12845,27 @@
       <c r="C168" s="121"/>
       <c r="D168" s="170">
         <f t="shared" si="85"/>
-        <v>0.43710063291139256</v>
+        <v>0.28650210970464107</v>
       </c>
       <c r="E168" s="170">
         <f t="shared" si="85"/>
-        <v>0.43710063291139251</v>
+        <v>0.30311603375527418</v>
       </c>
       <c r="F168" s="170">
         <f t="shared" si="85"/>
-        <v>0.43710063291139245</v>
+        <v>0.32665242616033746</v>
       </c>
       <c r="G168" s="170">
         <f t="shared" si="85"/>
-        <v>0.45608797468354428</v>
+        <v>0.34338172468354444</v>
       </c>
       <c r="H168" s="170">
         <f t="shared" si="85"/>
-        <v>0.45608797468354428</v>
+        <v>0.35039072389240511</v>
       </c>
       <c r="I168" s="171">
         <f t="shared" si="85"/>
-        <v>0.44383258402846243</v>
+        <v>0.31941361813840624</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -12885,31 +12885,31 @@
       </c>
       <c r="C171" s="177">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D171" s="117">
         <f>D$93-D$94-D$95-D$97-D$98-D$99-D$100-D$101-D$102-D$104</f>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="E171" s="117">
         <f t="shared" ref="E171:G171" si="86">E$93-E$94-E$95-E$97-E$98-E$99-E$100-E$101-E$102-E$104</f>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="F171" s="117">
         <f t="shared" si="86"/>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="G171" s="117">
         <f t="shared" si="86"/>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="H171" s="117">
         <f>H$93-H$94-H$95-H$97-H$98-H$99-H$100-H$101-H$102-H$104</f>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="I171" s="162">
         <f>NPV(_TauxDActualisation_Select,D171:H171)</f>
-        <v>159797442.65430853</v>
+        <v>140895718.91005415</v>
       </c>
       <c r="J171" s="182"/>
     </row>
@@ -12922,31 +12922,31 @@
       </c>
       <c r="C172" s="178">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D172" s="135">
         <f>D171*D$136</f>
-        <v>40022300.936045505</v>
+        <v>35288242.221857756</v>
       </c>
       <c r="E172" s="135">
         <f>E171*E$136</f>
-        <v>37057686.051893979</v>
+        <v>32674298.353571992</v>
       </c>
       <c r="F172" s="135">
         <f>F171*F$136</f>
-        <v>34312672.27027221</v>
+        <v>30253979.957011107</v>
       </c>
       <c r="G172" s="135">
         <f>G171*G$136</f>
-        <v>31770992.842844635</v>
+        <v>28012944.404639911</v>
       </c>
       <c r="H172" s="135">
         <f>H171*H$136</f>
-        <v>29417585.965596881</v>
+        <v>25937911.485777695</v>
       </c>
       <c r="I172" s="164">
         <f t="shared" ref="I172" si="87">SUM(D172:H172)</f>
-        <v>172581238.06665322</v>
+        <v>152167376.42285848</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
@@ -12971,31 +12971,31 @@
       </c>
       <c r="C175" s="127">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D175" s="117">
         <f>D$171-D141</f>
-        <v>29146274.430768754</v>
+        <v>27964368.557685871</v>
       </c>
       <c r="E175" s="117">
         <f t="shared" ref="E175:H175" si="88">E$171-E141</f>
-        <v>29146274.430768754</v>
+        <v>27461846.120982192</v>
       </c>
       <c r="F175" s="117">
         <f t="shared" si="88"/>
-        <v>29146274.430768754</v>
+        <v>26749939.335651994</v>
       </c>
       <c r="G175" s="117">
         <f t="shared" si="88"/>
-        <v>28555227.792472728</v>
+        <v>26243927.159804542</v>
       </c>
       <c r="H175" s="117">
         <f t="shared" si="88"/>
-        <v>28555227.792472728</v>
+        <v>26031925.506820187</v>
       </c>
       <c r="I175" s="162">
         <f>NPV(_TauxDActualisation_Select,C175:H175)</f>
-        <v>-10293446.235650498</v>
+        <v>-3696932.1305670151</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
@@ -13007,31 +13007,31 @@
       </c>
       <c r="C176" s="176">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D176" s="135">
         <f>D$172-D148</f>
-        <v>29146274.430768754</v>
+        <v>27964368.557685871</v>
       </c>
       <c r="E176" s="135">
         <f t="shared" ref="E176:H176" si="89">E$172-E148</f>
-        <v>26987291.139600694</v>
+        <v>25427635.297205731</v>
       </c>
       <c r="F176" s="135">
         <f t="shared" si="89"/>
-        <v>24988232.536667317</v>
+        <v>22933761.433172148</v>
       </c>
       <c r="G176" s="135">
         <f t="shared" si="89"/>
-        <v>22668060.471340053</v>
+        <v>20833275.510437734</v>
       </c>
       <c r="H176" s="135">
         <f t="shared" si="89"/>
-        <v>20988944.880870417</v>
+        <v>19134242.373286277</v>
       </c>
       <c r="I176" s="164">
         <f>SUM(C176:H176)</f>
-        <v>-1874047.6041879281</v>
+        <v>4621630.5709719136</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -13056,31 +13056,31 @@
       </c>
       <c r="C179" s="127">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D179" s="117">
         <f>D$171-D$145</f>
-        <v>22528527.866329797</v>
+        <v>25178086.377527118</v>
       </c>
       <c r="E179" s="117">
         <f>E$171-E$145</f>
-        <v>22528527.866329797</v>
+        <v>24591810.201372828</v>
       </c>
       <c r="F179" s="117">
         <f>F$171-F$145</f>
-        <v>22528527.866329797</v>
+        <v>23761252.285154261</v>
       </c>
       <c r="G179" s="117">
         <f>G$171-G$145</f>
-        <v>21768610.759949189</v>
+        <v>23170904.746665567</v>
       </c>
       <c r="H179" s="117">
         <f>H$171-H$145</f>
-        <v>21768610.759949189</v>
+        <v>22923569.484850481</v>
       </c>
       <c r="I179" s="162">
         <f>NPV(_TauxDActualisation_Select,C179:H179)</f>
-        <v>-34980296.577341169</v>
+        <v>-14611060.229661105</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -13092,31 +13092,31 @@
       </c>
       <c r="C180" s="176">
         <f>-(_CapitalSocial_Select+_DettesLT_Select+_DettesCT_Select+_DettesFournisseurs_Select)*_PIBPNB_Select</f>
-        <v>-126652851.06343517</v>
+        <v>-111671652.60081585</v>
       </c>
       <c r="D180" s="135">
         <f>D$172-D$152</f>
-        <v>22528527.866329797</v>
+        <v>25178086.377527118</v>
       </c>
       <c r="E180" s="135">
         <f>E$172-E$152</f>
-        <v>20859748.02437944</v>
+        <v>22770194.630900763</v>
       </c>
       <c r="F180" s="135">
         <f>F$172-F$152</f>
-        <v>19314581.504055042</v>
+        <v>20371444.003047206</v>
       </c>
       <c r="G180" s="135">
         <f>G$172-G$152</f>
-        <v>17280625.063466243</v>
+        <v>18393811.241510414</v>
       </c>
       <c r="H180" s="135">
         <f>H$172-H$152</f>
-        <v>16000578.762468742</v>
+        <v>16849507.90401892</v>
       </c>
       <c r="I180" s="164">
         <f>SUM(C180:H180)</f>
-        <v>-30668789.842735924</v>
+        <v>-8108608.4438114278</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
@@ -13151,11 +13151,11 @@
       </c>
       <c r="G183" s="179">
         <f>MAX(0,IRR($C171:G171))</f>
-        <v>0.1007746915436194</v>
+        <v>0.10077469154361873</v>
       </c>
       <c r="H183" s="180">
         <f>MAX(0,IRR($C171:H171))</f>
-        <v>0.17477335350611378</v>
+        <v>0.17477335350611312</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -13189,7 +13189,7 @@
       </c>
       <c r="H186" s="180">
         <f>MAX(0,IRR($C175:H175))</f>
-        <v>4.59346941356229E-2</v>
+        <v>6.6152872107589467E-2</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -13223,7 +13223,7 @@
       </c>
       <c r="H189" s="180">
         <f>MAX(0,IRR($C179:H179))</f>
-        <v>0</v>
+        <v>2.3786203374374537E-2</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
@@ -13257,7 +13257,7 @@
       </c>
       <c r="H192" s="180">
         <f t="shared" si="90"/>
-        <v>0.73717564368863553</v>
+        <v>0.62149337538873961</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -13291,7 +13291,7 @@
       </c>
       <c r="H195" s="180">
         <f>IF(H$183&gt;0,(H$183-H189)/H$183,0)</f>
-        <v>1</v>
+        <v>0.86390257497952883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
utilisation de l'api world banque
</commit_message>
<xml_diff>
--- a/annexe/Modèle investissement.xlsx
+++ b/annexe/Modèle investissement.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEE6F2F-5520-4C09-8124-3C0960EBCD64}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD24E688-9E47-4A2D-8180-7643C0E648BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="2" r:id="rId1"/>
@@ -2488,6 +2488,12 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2514,12 +2520,6 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2903,7 +2903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2929,19 +2929,19 @@
       <c r="B3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="216" t="s">
+      <c r="E3" s="218" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="217"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="214" t="s">
+      <c r="F3" s="219"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="216" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="215"/>
-      <c r="J3" s="214" t="s">
+      <c r="I3" s="217"/>
+      <c r="J3" s="216" t="s">
         <v>326</v>
       </c>
-      <c r="K3" s="215"/>
+      <c r="K3" s="217"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D4" s="190"/>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="I5" s="198">
         <f>Modèle!I163</f>
-        <v>3.3924050632911436E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
       <c r="J5" s="208"/>
       <c r="K5" s="209"/>
@@ -3019,19 +3019,19 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F69&lt;&gt;"",Select!G69&lt;&gt;""),Select!E69,""))</f>
         <v/>
       </c>
-      <c r="H6" s="219">
+      <c r="H6" s="221">
         <f>Modèle!D164</f>
         <v>0.2075443037974681</v>
       </c>
-      <c r="I6" s="221">
+      <c r="I6" s="223">
         <f>Modèle!I164</f>
-        <v>0.23575416816926681</v>
-      </c>
-      <c r="J6" s="219">
+        <v>0.23273122235010016</v>
+      </c>
+      <c r="J6" s="221">
         <f>Modèle!D192</f>
         <v>0</v>
       </c>
-      <c r="K6" s="221">
+      <c r="K6" s="223">
         <f>Modèle!H192</f>
         <v>0.62149337538873961</v>
       </c>
@@ -3060,10 +3060,10 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F70&lt;&gt;"",Select!G70&lt;&gt;""),Select!E70,""))</f>
         <v/>
       </c>
-      <c r="H7" s="220"/>
-      <c r="I7" s="222"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="222"/>
+      <c r="H7" s="222"/>
+      <c r="I7" s="224"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="224"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="56" t="str">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="I8" s="198">
         <f>Modèle!I165</f>
-        <v>3.9292361361544466E-2</v>
+        <v>3.8788537058350031E-2</v>
       </c>
       <c r="J8" s="208"/>
       <c r="K8" s="209"/>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="I11" s="174">
         <f>Modèle!I168</f>
-        <v>0.31941361813840624</v>
+        <v>0.31588684801604522</v>
       </c>
       <c r="J11" s="189">
         <f>Modèle!D195</f>
@@ -3200,15 +3200,15 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="223" t="str">
+      <c r="A16" s="214" t="str">
         <f>VLOOKUP(_Bilan,_Tables,4,FALSE)</f>
         <v>Bilan à l'ouverture</v>
       </c>
-      <c r="B16" s="223"/>
-      <c r="C16" s="223"/>
-      <c r="D16" s="223"/>
-      <c r="E16" s="223"/>
-      <c r="F16" s="223"/>
+      <c r="B16" s="214"/>
+      <c r="C16" s="214"/>
+      <c r="D16" s="214"/>
+      <c r="E16" s="214"/>
+      <c r="F16" s="214"/>
       <c r="H16" s="73" t="str">
         <f>VLOOKUP(_PIBPNB,_Tables,4,FALSE)</f>
         <v>PIB ou PNB</v>
@@ -3218,18 +3218,18 @@
       <c r="K16" s="68"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="224" t="str">
+      <c r="A17" s="215" t="str">
         <f>VLOOKUP(_Actif,_Tables,4,FALSE)</f>
         <v>Actif</v>
       </c>
-      <c r="B17" s="224"/>
-      <c r="C17" s="224"/>
-      <c r="D17" s="224" t="str">
+      <c r="B17" s="215"/>
+      <c r="C17" s="215"/>
+      <c r="D17" s="215" t="str">
         <f>VLOOKUP(_Passif,_Tables,4,FALSE)</f>
         <v>Passif</v>
       </c>
-      <c r="E17" s="224"/>
-      <c r="F17" s="224"/>
+      <c r="E17" s="215"/>
+      <c r="F17" s="215"/>
       <c r="H17" s="56" t="str">
         <f>_PIBPNB_Liste</f>
         <v>PIB/tête</v>
@@ -3529,34 +3529,34 @@
       <c r="I29" s="57"/>
       <c r="J29" s="78">
         <f>_TauxDActualisation_Select</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="70"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="223" t="str">
+      <c r="A31" s="214" t="str">
         <f>VLOOKUP(_CompteDeResultat,_Tables,4,FALSE)</f>
         <v>Compte de résultat</v>
       </c>
-      <c r="B31" s="223"/>
-      <c r="C31" s="223"/>
-      <c r="D31" s="223"/>
-      <c r="E31" s="223"/>
-      <c r="F31" s="223"/>
+      <c r="B31" s="214"/>
+      <c r="C31" s="214"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="224" t="str">
+      <c r="A32" s="215" t="str">
         <f>VLOOKUP(_Charges,_Tables,4,FALSE)</f>
         <v>Charges</v>
       </c>
-      <c r="B32" s="224"/>
-      <c r="C32" s="224"/>
-      <c r="D32" s="224" t="str">
+      <c r="B32" s="215"/>
+      <c r="C32" s="215"/>
+      <c r="D32" s="215" t="str">
         <f>VLOOKUP(_Produits,_Tables,4,FALSE)</f>
         <v>Produits</v>
       </c>
-      <c r="E32" s="224"/>
-      <c r="F32" s="224"/>
+      <c r="E32" s="215"/>
+      <c r="F32" s="215"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="str">
@@ -4072,12 +4072,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E3:G3"/>
@@ -4085,6 +4079,12 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="J28" s="1">
         <f>_TauxDActualisation_Select</f>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
@@ -4600,12 +4600,12 @@
       </c>
       <c r="C34" s="10">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="29">
         <f t="shared" si="1"/>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -9023,10 +9023,10 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9430,7 +9430,7 @@
         <v>_TauxDActualisation</v>
       </c>
       <c r="B56" s="10">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -9447,11 +9447,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12114,19 +12114,19 @@
       </c>
       <c r="E136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),1)</f>
-        <v>0.92592592592592582</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),2)</f>
-        <v>0.85733882030178321</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="G136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),3)</f>
-        <v>0.79383224102016958</v>
+        <v>0.57870370370370372</v>
       </c>
       <c r="H136" s="161">
         <f>1/POWER((1+_TauxDActualisation_Select),4)</f>
-        <v>0.73502985279645328</v>
+        <v>0.48225308641975312</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
@@ -12175,7 +12175,7 @@
       </c>
       <c r="I140" s="162">
         <f>NPV(_TauxDActualisation_Select,D140:H140)</f>
-        <v>4779753.502265133</v>
+        <v>3580121.9514926379</v>
       </c>
       <c r="K140" s="182">
         <f>(D140/(1.08))+(D140/(1.08*2))+(D140/(1.08*3))+(D140/(1.08*4))+(D140/(1.08*5))</f>
@@ -12212,7 +12212,7 @@
       </c>
       <c r="I141" s="163">
         <f t="shared" ref="I141:I145" si="71">NPV(_TauxDActualisation_Select,D141:H141)</f>
-        <v>33216753.010250647</v>
+        <v>24560927.789825071</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
@@ -12245,7 +12245,7 @@
       </c>
       <c r="I142" s="163">
         <f t="shared" si="71"/>
-        <v>5536125.5017084414</v>
+        <v>4093487.9649708462</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
@@ -12278,7 +12278,7 @@
       </c>
       <c r="I143" s="163">
         <f t="shared" si="71"/>
-        <v>1471379.3430480356</v>
+        <v>1102089.7798438156</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
@@ -12344,7 +12344,7 @@
       </c>
       <c r="I145" s="165">
         <f t="shared" si="71"/>
-        <v>45004011.35727226</v>
+        <v>33336627.486132372</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -12369,23 +12369,23 @@
       </c>
       <c r="E147" s="117">
         <f t="shared" si="75"/>
-        <v>1108444.5517414312</v>
+        <v>997600.09656728827</v>
       </c>
       <c r="F147" s="117">
         <f t="shared" si="75"/>
-        <v>1026337.5479087328</v>
+        <v>831333.41380607348</v>
       </c>
       <c r="G147" s="117">
         <f t="shared" si="75"/>
-        <v>950312.54435993766</v>
+        <v>692777.84483839467</v>
       </c>
       <c r="H147" s="117">
         <f t="shared" si="75"/>
-        <v>879919.02255549782</v>
+        <v>577314.87069866224</v>
       </c>
       <c r="I147" s="162">
         <f>SUM(D147:H147)</f>
-        <v>5162133.7824463444</v>
+        <v>4296146.3417911651</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -12402,23 +12402,23 @@
       </c>
       <c r="E148" s="113">
         <f t="shared" si="75"/>
-        <v>7246663.0563662602</v>
+        <v>6521996.7507296354</v>
       </c>
       <c r="F148" s="113">
         <f t="shared" si="75"/>
-        <v>7320218.5238389596</v>
+        <v>5929377.0043095574</v>
       </c>
       <c r="G148" s="113">
         <f t="shared" si="75"/>
-        <v>7179668.8942021774</v>
+        <v>5233978.6238733884</v>
       </c>
       <c r="H148" s="113">
         <f t="shared" si="75"/>
-        <v>6803669.1124914158</v>
+        <v>4463887.3047056189</v>
       </c>
       <c r="I148" s="163">
         <f t="shared" ref="I148:I152" si="76">SUM(D148:H148)</f>
-        <v>35874093.251070701</v>
+        <v>29473113.347790085</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -12435,23 +12435,23 @@
       </c>
       <c r="E149" s="113">
         <f>E142*E$136</f>
-        <v>1207777.1760610435</v>
+        <v>1086999.4584549393</v>
       </c>
       <c r="F149" s="113">
         <f t="shared" si="77"/>
-        <v>1220036.4206398265</v>
+        <v>988229.50071825949</v>
       </c>
       <c r="G149" s="113">
         <f t="shared" si="77"/>
-        <v>1196611.4823670299</v>
+        <v>872329.77064556489</v>
       </c>
       <c r="H149" s="113">
         <f t="shared" si="77"/>
-        <v>1133944.8520819028</v>
+        <v>743981.21745093667</v>
       </c>
       <c r="I149" s="163">
         <f t="shared" si="76"/>
-        <v>5979015.5418451168</v>
+        <v>4912185.5579650151</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -12468,23 +12468,23 @@
       </c>
       <c r="E150" s="113">
         <f t="shared" si="78"/>
-        <v>341218.93850249285</v>
+        <v>307097.04465224361</v>
       </c>
       <c r="F150" s="113">
         <f t="shared" si="78"/>
-        <v>315943.46157638228</v>
+        <v>255914.20387686964</v>
       </c>
       <c r="G150" s="113">
         <f t="shared" si="78"/>
-        <v>292540.24220035394</v>
+        <v>213261.83656405806</v>
       </c>
       <c r="H150" s="113">
         <f t="shared" si="78"/>
-        <v>270870.59462995734</v>
+        <v>177718.19713671505</v>
       </c>
       <c r="I150" s="163">
         <f t="shared" si="76"/>
-        <v>1589089.6904918787</v>
+        <v>1322507.7358125786</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -12534,23 +12534,23 @@
       </c>
       <c r="E152" s="122">
         <f t="shared" ref="E152" si="80">SUM(E147:E151)</f>
-        <v>9904103.7226712275</v>
+        <v>8913693.3504041061</v>
       </c>
       <c r="F152" s="122">
         <f t="shared" ref="F152" si="81">SUM(F147:F151)</f>
-        <v>9882535.9539639</v>
+        <v>8004854.1227107598</v>
       </c>
       <c r="G152" s="122">
         <f t="shared" ref="G152" si="82">SUM(G147:G151)</f>
-        <v>9619133.1631294992</v>
+        <v>7012348.075921407</v>
       </c>
       <c r="H152" s="122">
         <f t="shared" ref="H152" si="83">SUM(H147:H151)</f>
-        <v>9088403.5817587748</v>
+        <v>5962901.5899919327</v>
       </c>
       <c r="I152" s="165">
         <f t="shared" si="76"/>
-        <v>48604332.265854038</v>
+        <v>40003952.983358845</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -12593,7 +12593,7 @@
       </c>
       <c r="I156" s="168">
         <f t="shared" si="84"/>
-        <v>3.3924050632911429E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -12626,7 +12626,7 @@
       </c>
       <c r="I157" s="169">
         <f>I141/I$171</f>
-        <v>0.23575416816926678</v>
+        <v>0.23273122235010013</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -12659,7 +12659,7 @@
       </c>
       <c r="I158" s="169">
         <f t="shared" si="84"/>
-        <v>3.9292361361544466E-2</v>
+        <v>3.8788537058350031E-2</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -12692,7 +12692,7 @@
       </c>
       <c r="I159" s="169">
         <f t="shared" si="84"/>
-        <v>1.0443037974683557E-2</v>
+        <v>1.0443037974683558E-2</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -12758,7 +12758,7 @@
       </c>
       <c r="I161" s="171">
         <f t="shared" si="84"/>
-        <v>0.31941361813840624</v>
+        <v>0.31588684801604516</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
@@ -12796,7 +12796,7 @@
       </c>
       <c r="I163" s="168">
         <f t="shared" si="85"/>
-        <v>3.3924050632911436E-2</v>
+        <v>3.3924050632911443E-2</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
@@ -12813,7 +12813,7 @@
       </c>
       <c r="E164" s="167">
         <f t="shared" si="85"/>
-        <v>0.22178481012658216</v>
+        <v>0.22178481012658213</v>
       </c>
       <c r="F164" s="167">
         <f t="shared" si="85"/>
@@ -12829,7 +12829,7 @@
       </c>
       <c r="I164" s="169">
         <f t="shared" si="85"/>
-        <v>0.23575416816926681</v>
+        <v>0.23273122235010016</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -12854,15 +12854,15 @@
       </c>
       <c r="G165" s="167">
         <f t="shared" si="85"/>
-        <v>4.2716376582278504E-2</v>
+        <v>4.2716376582278497E-2</v>
       </c>
       <c r="H165" s="167">
         <f t="shared" si="85"/>
-        <v>4.3717662183544295E-2</v>
+        <v>4.3717662183544302E-2</v>
       </c>
       <c r="I165" s="169">
         <f t="shared" si="85"/>
-        <v>3.9292361361544466E-2</v>
+        <v>3.8788537058350031E-2</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
@@ -12883,7 +12883,7 @@
       </c>
       <c r="F166" s="167">
         <f t="shared" si="85"/>
-        <v>1.044303797468356E-2</v>
+        <v>1.0443037974683558E-2</v>
       </c>
       <c r="G166" s="167">
         <f t="shared" si="85"/>
@@ -12953,15 +12953,15 @@
       </c>
       <c r="G168" s="170">
         <f t="shared" si="85"/>
-        <v>0.34338172468354444</v>
+        <v>0.3433817246835445</v>
       </c>
       <c r="H168" s="170">
         <f t="shared" si="85"/>
-        <v>0.35039072389240511</v>
+        <v>0.35039072389240505</v>
       </c>
       <c r="I168" s="171">
         <f t="shared" si="85"/>
-        <v>0.31941361813840624</v>
+        <v>0.31588684801604522</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -13005,7 +13005,7 @@
       </c>
       <c r="I171" s="162">
         <f>NPV(_TauxDActualisation_Select,D171:H171)</f>
-        <v>140895718.91005415</v>
+        <v>105533445.58504401</v>
       </c>
       <c r="J171" s="182"/>
     </row>
@@ -13026,23 +13026,23 @@
       </c>
       <c r="E172" s="135">
         <f>E171*E$136</f>
-        <v>32674298.353571992</v>
+        <v>29406868.518214799</v>
       </c>
       <c r="F172" s="135">
         <f>F171*F$136</f>
-        <v>30253979.957011107</v>
+        <v>24505723.765178997</v>
       </c>
       <c r="G172" s="135">
         <f>G171*G$136</f>
-        <v>28012944.404639911</v>
+        <v>20421436.470982499</v>
       </c>
       <c r="H172" s="135">
         <f>H171*H$136</f>
-        <v>25937911.485777695</v>
+        <v>17017863.72581875</v>
       </c>
       <c r="I172" s="164">
         <f t="shared" ref="I172" si="87">SUM(D172:H172)</f>
-        <v>152167376.42285848</v>
+        <v>126640134.7020528</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
@@ -13091,7 +13091,7 @@
       </c>
       <c r="I175" s="162">
         <f>NPV(_TauxDActualisation_Select,C175:H175)</f>
-        <v>-3696932.1305670151</v>
+        <v>-25582612.337997433</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
@@ -13111,23 +13111,23 @@
       </c>
       <c r="E176" s="135">
         <f t="shared" ref="E176:H176" si="89">E$172-E148</f>
-        <v>25427635.297205731</v>
+        <v>22884871.767485164</v>
       </c>
       <c r="F176" s="135">
         <f t="shared" si="89"/>
-        <v>22933761.433172148</v>
+        <v>18576346.76086944</v>
       </c>
       <c r="G176" s="135">
         <f t="shared" si="89"/>
-        <v>20833275.510437734</v>
+        <v>15187457.847109111</v>
       </c>
       <c r="H176" s="135">
         <f t="shared" si="89"/>
-        <v>19134242.373286277</v>
+        <v>12553976.42111313</v>
       </c>
       <c r="I176" s="164">
         <f>SUM(C176:H176)</f>
-        <v>4621630.5709719136</v>
+        <v>-14504631.246553142</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="I179" s="162">
         <f>NPV(_TauxDActualisation_Select,C179:H179)</f>
-        <v>-14611060.229661105</v>
+        <v>-32895695.418253522</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -13196,23 +13196,23 @@
       </c>
       <c r="E180" s="135">
         <f>E$172-E$152</f>
-        <v>22770194.630900763</v>
+        <v>20493175.167810693</v>
       </c>
       <c r="F180" s="135">
         <f>F$172-F$152</f>
-        <v>20371444.003047206</v>
+        <v>16500869.642468236</v>
       </c>
       <c r="G180" s="135">
         <f>G$172-G$152</f>
-        <v>18393811.241510414</v>
+        <v>13409088.395061092</v>
       </c>
       <c r="H180" s="135">
         <f>H$172-H$152</f>
-        <v>16849507.90401892</v>
+        <v>11054962.135826817</v>
       </c>
       <c r="I180" s="164">
         <f>SUM(C180:H180)</f>
-        <v>-8108608.4438114278</v>
+        <v>-25035470.882121891</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
quelque test à faire, un code à mettre au propre, debut des graphes a faire installation d une bibliothéque pour graphique
</commit_message>
<xml_diff>
--- a/annexe/Modèle investissement.xlsx
+++ b/annexe/Modèle investissement.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD24E688-9E47-4A2D-8180-7643C0E648BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C5A93-62BC-4CDE-A8C5-0225D887704E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="2" r:id="rId1"/>
@@ -2488,38 +2488,38 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2901,10 +2901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2912,7 +2912,7 @@
     <col min="1" max="16384" width="12.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>240</v>
       </c>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="I1" s="34"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>VLOOKUP(_Donnee,_Tables,4,FALSE)</f>
         <v>Données</v>
@@ -2929,21 +2929,21 @@
       <c r="B3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="218" t="s">
+      <c r="E3" s="216" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="219"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="216" t="s">
+      <c r="F3" s="217"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="214" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="217"/>
-      <c r="J3" s="216" t="s">
+      <c r="I3" s="215"/>
+      <c r="J3" s="214" t="s">
         <v>326</v>
       </c>
-      <c r="K3" s="217"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="215"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D4" s="190"/>
       <c r="E4" s="191" t="s">
         <v>319</v>
@@ -2967,7 +2967,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>VLOOKUP(_PIBPNB,_Tables,4,FALSE)</f>
         <v>PIB ou PNB</v>
@@ -2997,12 +2997,12 @@
       </c>
       <c r="I5" s="198">
         <f>Modèle!I163</f>
-        <v>3.3924050632911443E-2</v>
+        <v>3.3924050632911436E-2</v>
       </c>
       <c r="J5" s="208"/>
       <c r="K5" s="209"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D6" s="199" t="str">
         <f>VLOOKUP(CONCATENATE(_Impot,_Impot_IS),_Tables,3,FALSE)</f>
         <v>IS</v>
@@ -3019,24 +3019,24 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F69&lt;&gt;"",Select!G69&lt;&gt;""),Select!E69,""))</f>
         <v/>
       </c>
-      <c r="H6" s="221">
+      <c r="H6" s="219">
         <f>Modèle!D164</f>
         <v>0.2075443037974681</v>
       </c>
-      <c r="I6" s="223">
+      <c r="I6" s="221">
         <f>Modèle!I164</f>
-        <v>0.23273122235010016</v>
-      </c>
-      <c r="J6" s="221">
+        <v>0.23575416816926681</v>
+      </c>
+      <c r="J6" s="219">
         <f>Modèle!D192</f>
         <v>0</v>
       </c>
-      <c r="K6" s="223">
+      <c r="K6" s="221">
         <f>Modèle!H192</f>
         <v>0.62149337538873961</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>VLOOKUP(_Pays,_Tables,4,FALSE)</f>
         <v>Pays</v>
@@ -3060,12 +3060,12 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F70&lt;&gt;"",Select!G70&lt;&gt;""),Select!E70,""))</f>
         <v/>
       </c>
-      <c r="H7" s="222"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="222"/>
-      <c r="K7" s="224"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="220"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="222"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D8" s="56" t="str">
         <f>VLOOKUP(CONCATENATE(_Impot,_Impot_IRVM),_Tables,3,FALSE)</f>
         <v>IRVM</v>
@@ -3088,12 +3088,12 @@
       </c>
       <c r="I8" s="198">
         <f>Modèle!I165</f>
-        <v>3.8788537058350031E-2</v>
+        <v>3.9292361361544466E-2</v>
       </c>
       <c r="J8" s="208"/>
       <c r="K8" s="209"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>VLOOKUP(_Regime,_Tables,4,FALSE)</f>
         <v>Régime</v>
@@ -3128,7 +3128,7 @@
       <c r="J9" s="210"/>
       <c r="K9" s="211"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="str">
         <f>Select!B62</f>
         <v/>
@@ -3160,7 +3160,7 @@
       <c r="J10" s="208"/>
       <c r="K10" s="209"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="str">
         <f>Select!B63</f>
         <v/>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="I11" s="174">
         <f>Modèle!I168</f>
-        <v>0.31588684801604522</v>
+        <v>0.31941361813840624</v>
       </c>
       <c r="J11" s="189">
         <f>Modèle!D195</f>
@@ -3188,27 +3188,35 @@
         <v>0.86390257497952883</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="str">
         <f>Select!B64</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N13" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="214" t="str">
+      <c r="N14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="223" t="str">
         <f>VLOOKUP(_Bilan,_Tables,4,FALSE)</f>
         <v>Bilan à l'ouverture</v>
       </c>
-      <c r="B16" s="214"/>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="214"/>
+      <c r="B16" s="223"/>
+      <c r="C16" s="223"/>
+      <c r="D16" s="223"/>
+      <c r="E16" s="223"/>
+      <c r="F16" s="223"/>
       <c r="H16" s="73" t="str">
         <f>VLOOKUP(_PIBPNB,_Tables,4,FALSE)</f>
         <v>PIB ou PNB</v>
@@ -3217,19 +3225,19 @@
       <c r="J16" s="67"/>
       <c r="K16" s="68"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="215" t="str">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="224" t="str">
         <f>VLOOKUP(_Actif,_Tables,4,FALSE)</f>
         <v>Actif</v>
       </c>
-      <c r="B17" s="215"/>
-      <c r="C17" s="215"/>
-      <c r="D17" s="215" t="str">
+      <c r="B17" s="224"/>
+      <c r="C17" s="224"/>
+      <c r="D17" s="224" t="str">
         <f>VLOOKUP(_Passif,_Tables,4,FALSE)</f>
         <v>Passif</v>
       </c>
-      <c r="E17" s="215"/>
-      <c r="F17" s="215"/>
+      <c r="E17" s="224"/>
+      <c r="F17" s="224"/>
       <c r="H17" s="56" t="str">
         <f>_PIBPNB_Liste</f>
         <v>PIB/tête</v>
@@ -3243,7 +3251,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="str">
         <f>VLOOKUP(_ActifImmo,_Tables,4,FALSE)</f>
         <v>Actif immobilisé</v>
@@ -3256,8 +3264,12 @@
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="37"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N18" s="1">
+        <f>F34/(1+N13)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="str">
         <f>VLOOKUP(_Terrain,_Tables,4,FALSE)</f>
         <v>Terrain</v>
@@ -3284,7 +3296,7 @@
       <c r="J19" s="67"/>
       <c r="K19" s="68"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="str">
         <f>VLOOKUP(_Constructions,_Tables,4,FALSE)</f>
         <v>Constructions</v>
@@ -3308,7 +3320,7 @@
         <v>Indice salarial</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="str">
         <f>VLOOKUP(_Equipement,_Tables,4,FALSE)</f>
         <v>Equipement</v>
@@ -3335,7 +3347,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="str">
         <f>VLOOKUP(_Camion,_Tables,4,FALSE)</f>
         <v>Camion</v>
@@ -3362,7 +3374,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="str">
         <f>VLOOKUP(_Informatique,_Tables,4,FALSE)</f>
         <v>Matériel informatique</v>
@@ -3389,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="str">
         <f>VLOOKUP(_Bureau,_Tables,4,FALSE)</f>
         <v>Matériel de bureau</v>
@@ -3403,7 +3415,7 @@
       <c r="E24" s="46"/>
       <c r="F24" s="49"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="61" t="str">
         <f>VLOOKUP(_ActifCirculant,_Tables,4,FALSE)</f>
         <v>Actif circulant</v>
@@ -3424,7 +3436,7 @@
       <c r="J25" s="67"/>
       <c r="K25" s="68"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="str">
         <f>VLOOKUP(_Stocks,_Tables,4,FALSE)</f>
         <v>Stocks</v>
@@ -3456,7 +3468,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="str">
         <f>VLOOKUP(_CreancesClients,_Tables,4,FALSE)</f>
         <v>Créances clients</v>
@@ -3476,7 +3488,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="str">
         <f>VLOOKUP(_DisponibilitesBancaires,_Tables,4,FALSE)</f>
         <v>Disponibilités bancaires</v>
@@ -3503,7 +3515,7 @@
       <c r="J28" s="67"/>
       <c r="K28" s="68"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="63" t="str">
         <f>VLOOKUP(_Actif,_Tables,4,FALSE)</f>
         <v>Actif</v>
@@ -3529,34 +3541,34 @@
       <c r="I29" s="57"/>
       <c r="J29" s="78">
         <f>_TauxDActualisation_Select</f>
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="K29" s="70"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="214" t="str">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="223" t="str">
         <f>VLOOKUP(_CompteDeResultat,_Tables,4,FALSE)</f>
         <v>Compte de résultat</v>
       </c>
-      <c r="B31" s="214"/>
-      <c r="C31" s="214"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="214"/>
-      <c r="F31" s="214"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="215" t="str">
+      <c r="B31" s="223"/>
+      <c r="C31" s="223"/>
+      <c r="D31" s="223"/>
+      <c r="E31" s="223"/>
+      <c r="F31" s="223"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="224" t="str">
         <f>VLOOKUP(_Charges,_Tables,4,FALSE)</f>
         <v>Charges</v>
       </c>
-      <c r="B32" s="215"/>
-      <c r="C32" s="215"/>
-      <c r="D32" s="215" t="str">
+      <c r="B32" s="224"/>
+      <c r="C32" s="224"/>
+      <c r="D32" s="224" t="str">
         <f>VLOOKUP(_Produits,_Tables,4,FALSE)</f>
         <v>Produits</v>
       </c>
-      <c r="E32" s="215"/>
-      <c r="F32" s="215"/>
+      <c r="E32" s="224"/>
+      <c r="F32" s="224"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="str">
@@ -4072,6 +4084,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E3:G3"/>
@@ -4079,12 +4097,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4519,7 +4531,7 @@
       </c>
       <c r="J28" s="1">
         <f>_TauxDActualisation_Select</f>
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
@@ -4600,12 +4612,12 @@
       </c>
       <c r="C34" s="10">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="29">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -5583,7 +5595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D114"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7134,7 +7148,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="R36" sqref="R36"/>
@@ -9026,7 +9040,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
+      <selection pane="bottomRight" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9430,7 +9444,7 @@
         <v>_TauxDActualisation</v>
       </c>
       <c r="B56" s="10">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>
@@ -9445,13 +9459,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M195"/>
+  <dimension ref="A1:O195"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C176" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C178" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D115" sqref="D115"/>
+      <selection pane="bottomRight" activeCell="R203" sqref="R203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11917,6 +11931,10 @@
         <f t="shared" si="66"/>
         <v>30854389.050125241</v>
       </c>
+      <c r="I126" s="182">
+        <f>D110-D125</f>
+        <v>17089038.549734402</v>
+      </c>
       <c r="M126" s="1">
         <v>-10000</v>
       </c>
@@ -12114,19 +12132,19 @@
       </c>
       <c r="E136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),1)</f>
-        <v>0.83333333333333337</v>
+        <v>0.92592592592592582</v>
       </c>
       <c r="F136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),2)</f>
-        <v>0.69444444444444442</v>
+        <v>0.85733882030178321</v>
       </c>
       <c r="G136" s="160">
         <f>1/POWER((1+_TauxDActualisation_Select),3)</f>
-        <v>0.57870370370370372</v>
+        <v>0.79383224102016958</v>
       </c>
       <c r="H136" s="161">
         <f>1/POWER((1+_TauxDActualisation_Select),4)</f>
-        <v>0.48225308641975312</v>
+        <v>0.73502985279645328</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
@@ -12175,7 +12193,7 @@
       </c>
       <c r="I140" s="162">
         <f>NPV(_TauxDActualisation_Select,D140:H140)</f>
-        <v>3580121.9514926379</v>
+        <v>4779753.502265133</v>
       </c>
       <c r="K140" s="182">
         <f>(D140/(1.08))+(D140/(1.08*2))+(D140/(1.08*3))+(D140/(1.08*4))+(D140/(1.08*5))</f>
@@ -12212,7 +12230,7 @@
       </c>
       <c r="I141" s="163">
         <f t="shared" ref="I141:I145" si="71">NPV(_TauxDActualisation_Select,D141:H141)</f>
-        <v>24560927.789825071</v>
+        <v>33216753.010250647</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
@@ -12245,7 +12263,7 @@
       </c>
       <c r="I142" s="163">
         <f t="shared" si="71"/>
-        <v>4093487.9649708462</v>
+        <v>5536125.5017084414</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
@@ -12278,7 +12296,7 @@
       </c>
       <c r="I143" s="163">
         <f t="shared" si="71"/>
-        <v>1102089.7798438156</v>
+        <v>1471379.3430480356</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
@@ -12344,7 +12362,7 @@
       </c>
       <c r="I145" s="165">
         <f t="shared" si="71"/>
-        <v>33336627.486132372</v>
+        <v>45004011.35727226</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -12369,23 +12387,23 @@
       </c>
       <c r="E147" s="117">
         <f t="shared" si="75"/>
-        <v>997600.09656728827</v>
+        <v>1108444.5517414312</v>
       </c>
       <c r="F147" s="117">
         <f t="shared" si="75"/>
-        <v>831333.41380607348</v>
+        <v>1026337.5479087328</v>
       </c>
       <c r="G147" s="117">
         <f t="shared" si="75"/>
-        <v>692777.84483839467</v>
+        <v>950312.54435993766</v>
       </c>
       <c r="H147" s="117">
         <f t="shared" si="75"/>
-        <v>577314.87069866224</v>
+        <v>879919.02255549782</v>
       </c>
       <c r="I147" s="162">
         <f>SUM(D147:H147)</f>
-        <v>4296146.3417911651</v>
+        <v>5162133.7824463444</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -12402,23 +12420,23 @@
       </c>
       <c r="E148" s="113">
         <f t="shared" si="75"/>
-        <v>6521996.7507296354</v>
+        <v>7246663.0563662602</v>
       </c>
       <c r="F148" s="113">
         <f t="shared" si="75"/>
-        <v>5929377.0043095574</v>
+        <v>7320218.5238389596</v>
       </c>
       <c r="G148" s="113">
         <f t="shared" si="75"/>
-        <v>5233978.6238733884</v>
+        <v>7179668.8942021774</v>
       </c>
       <c r="H148" s="113">
         <f t="shared" si="75"/>
-        <v>4463887.3047056189</v>
+        <v>6803669.1124914158</v>
       </c>
       <c r="I148" s="163">
         <f t="shared" ref="I148:I152" si="76">SUM(D148:H148)</f>
-        <v>29473113.347790085</v>
+        <v>35874093.251070701</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -12435,23 +12453,23 @@
       </c>
       <c r="E149" s="113">
         <f>E142*E$136</f>
-        <v>1086999.4584549393</v>
+        <v>1207777.1760610435</v>
       </c>
       <c r="F149" s="113">
         <f t="shared" si="77"/>
-        <v>988229.50071825949</v>
+        <v>1220036.4206398265</v>
       </c>
       <c r="G149" s="113">
         <f t="shared" si="77"/>
-        <v>872329.77064556489</v>
+        <v>1196611.4823670299</v>
       </c>
       <c r="H149" s="113">
         <f t="shared" si="77"/>
-        <v>743981.21745093667</v>
+        <v>1133944.8520819028</v>
       </c>
       <c r="I149" s="163">
         <f t="shared" si="76"/>
-        <v>4912185.5579650151</v>
+        <v>5979015.5418451168</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -12468,23 +12486,23 @@
       </c>
       <c r="E150" s="113">
         <f t="shared" si="78"/>
-        <v>307097.04465224361</v>
+        <v>341218.93850249285</v>
       </c>
       <c r="F150" s="113">
         <f t="shared" si="78"/>
-        <v>255914.20387686964</v>
+        <v>315943.46157638228</v>
       </c>
       <c r="G150" s="113">
         <f t="shared" si="78"/>
-        <v>213261.83656405806</v>
+        <v>292540.24220035394</v>
       </c>
       <c r="H150" s="113">
         <f t="shared" si="78"/>
-        <v>177718.19713671505</v>
+        <v>270870.59462995734</v>
       </c>
       <c r="I150" s="163">
         <f t="shared" si="76"/>
-        <v>1322507.7358125786</v>
+        <v>1589089.6904918787</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -12534,23 +12552,23 @@
       </c>
       <c r="E152" s="122">
         <f t="shared" ref="E152" si="80">SUM(E147:E151)</f>
-        <v>8913693.3504041061</v>
+        <v>9904103.7226712275</v>
       </c>
       <c r="F152" s="122">
         <f t="shared" ref="F152" si="81">SUM(F147:F151)</f>
-        <v>8004854.1227107598</v>
+        <v>9882535.9539639</v>
       </c>
       <c r="G152" s="122">
         <f t="shared" ref="G152" si="82">SUM(G147:G151)</f>
-        <v>7012348.075921407</v>
+        <v>9619133.1631294992</v>
       </c>
       <c r="H152" s="122">
         <f t="shared" ref="H152" si="83">SUM(H147:H151)</f>
-        <v>5962901.5899919327</v>
+        <v>9088403.5817587748</v>
       </c>
       <c r="I152" s="165">
         <f t="shared" si="76"/>
-        <v>40003952.983358845</v>
+        <v>48604332.265854038</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -12593,7 +12611,7 @@
       </c>
       <c r="I156" s="168">
         <f t="shared" si="84"/>
-        <v>3.3924050632911443E-2</v>
+        <v>3.3924050632911429E-2</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -12626,7 +12644,7 @@
       </c>
       <c r="I157" s="169">
         <f>I141/I$171</f>
-        <v>0.23273122235010013</v>
+        <v>0.23575416816926678</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -12659,7 +12677,7 @@
       </c>
       <c r="I158" s="169">
         <f t="shared" si="84"/>
-        <v>3.8788537058350031E-2</v>
+        <v>3.9292361361544466E-2</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -12692,7 +12710,7 @@
       </c>
       <c r="I159" s="169">
         <f t="shared" si="84"/>
-        <v>1.0443037974683558E-2</v>
+        <v>1.0443037974683557E-2</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -12728,7 +12746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" s="108" t="s">
         <v>267</v>
       </c>
@@ -12758,15 +12776,15 @@
       </c>
       <c r="I161" s="171">
         <f t="shared" si="84"/>
-        <v>0.31588684801604516</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.31941361813840624</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" s="147" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" s="115" t="s">
         <v>54</v>
       </c>
@@ -12796,10 +12814,10 @@
       </c>
       <c r="I163" s="168">
         <f t="shared" si="85"/>
-        <v>3.3924050632911443E-2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.3924050632911436E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" s="101" t="s">
         <v>288</v>
       </c>
@@ -12813,7 +12831,7 @@
       </c>
       <c r="E164" s="167">
         <f t="shared" si="85"/>
-        <v>0.22178481012658213</v>
+        <v>0.22178481012658216</v>
       </c>
       <c r="F164" s="167">
         <f t="shared" si="85"/>
@@ -12829,10 +12847,10 @@
       </c>
       <c r="I164" s="169">
         <f t="shared" si="85"/>
-        <v>0.23273122235010016</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.23575416816926681</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" s="101" t="s">
         <v>59</v>
       </c>
@@ -12854,18 +12872,18 @@
       </c>
       <c r="G165" s="167">
         <f t="shared" si="85"/>
-        <v>4.2716376582278497E-2</v>
+        <v>4.2716376582278504E-2</v>
       </c>
       <c r="H165" s="167">
         <f t="shared" si="85"/>
-        <v>4.3717662183544302E-2</v>
+        <v>4.3717662183544295E-2</v>
       </c>
       <c r="I165" s="169">
         <f t="shared" si="85"/>
-        <v>3.8788537058350031E-2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.9292361361544466E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" s="101" t="s">
         <v>60</v>
       </c>
@@ -12883,7 +12901,7 @@
       </c>
       <c r="F166" s="167">
         <f t="shared" si="85"/>
-        <v>1.0443037974683558E-2</v>
+        <v>1.044303797468356E-2</v>
       </c>
       <c r="G166" s="167">
         <f t="shared" si="85"/>
@@ -12898,7 +12916,7 @@
         <v>1.0443037974683558E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" s="101" t="s">
         <v>61</v>
       </c>
@@ -12931,7 +12949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" s="108" t="s">
         <v>267</v>
       </c>
@@ -12953,26 +12971,44 @@
       </c>
       <c r="G168" s="170">
         <f t="shared" si="85"/>
-        <v>0.3433817246835445</v>
+        <v>0.34338172468354444</v>
       </c>
       <c r="H168" s="170">
         <f t="shared" si="85"/>
-        <v>0.35039072389240505</v>
+        <v>0.35039072389240511</v>
       </c>
       <c r="I168" s="171">
         <f t="shared" si="85"/>
-        <v>0.31588684801604522</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.31941361813840624</v>
+      </c>
+      <c r="N168" s="1">
+        <f>2^4</f>
+        <v>16</v>
+      </c>
+      <c r="O168" s="1">
+        <f>2^5</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O169" s="1">
+        <f>2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" s="152" t="s">
         <v>301</v>
       </c>
       <c r="I170" s="6" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="O170" s="1">
+        <f>(4/2)^4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" s="96" t="s">
         <v>291</v>
       </c>
@@ -13005,11 +13041,15 @@
       </c>
       <c r="I171" s="162">
         <f>NPV(_TauxDActualisation_Select,D171:H171)</f>
-        <v>105533445.58504401</v>
+        <v>140895718.91005415</v>
       </c>
       <c r="J171" s="182"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="O171" s="1">
+        <f>4^4/2^4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" s="149" t="s">
         <v>300</v>
       </c>
@@ -13026,31 +13066,31 @@
       </c>
       <c r="E172" s="135">
         <f>E171*E$136</f>
-        <v>29406868.518214799</v>
+        <v>32674298.353571992</v>
       </c>
       <c r="F172" s="135">
         <f>F171*F$136</f>
-        <v>24505723.765178997</v>
+        <v>30253979.957011107</v>
       </c>
       <c r="G172" s="135">
         <f>G171*G$136</f>
-        <v>20421436.470982499</v>
+        <v>28012944.404639911</v>
       </c>
       <c r="H172" s="135">
         <f>H171*H$136</f>
-        <v>17017863.72581875</v>
+        <v>25937911.485777695</v>
       </c>
       <c r="I172" s="164">
         <f t="shared" ref="I172" si="87">SUM(D172:H172)</f>
-        <v>126640134.7020528</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+        <v>152167376.42285848</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I173" s="6" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" s="152" t="s">
         <v>314</v>
       </c>
@@ -13058,7 +13098,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="96" t="s">
         <v>291</v>
       </c>
@@ -13091,10 +13131,10 @@
       </c>
       <c r="I175" s="162">
         <f>NPV(_TauxDActualisation_Select,C175:H175)</f>
-        <v>-25582612.337997433</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-3696932.1305670151</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" s="149" t="s">
         <v>300</v>
       </c>
@@ -13111,23 +13151,23 @@
       </c>
       <c r="E176" s="135">
         <f t="shared" ref="E176:H176" si="89">E$172-E148</f>
-        <v>22884871.767485164</v>
+        <v>25427635.297205731</v>
       </c>
       <c r="F176" s="135">
         <f t="shared" si="89"/>
-        <v>18576346.76086944</v>
+        <v>22933761.433172148</v>
       </c>
       <c r="G176" s="135">
         <f t="shared" si="89"/>
-        <v>15187457.847109111</v>
+        <v>20833275.510437734</v>
       </c>
       <c r="H176" s="135">
         <f t="shared" si="89"/>
-        <v>12553976.42111313</v>
+        <v>19134242.373286277</v>
       </c>
       <c r="I176" s="164">
         <f>SUM(C176:H176)</f>
-        <v>-14504631.246553142</v>
+        <v>4621630.5709719136</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -13176,7 +13216,7 @@
       </c>
       <c r="I179" s="162">
         <f>NPV(_TauxDActualisation_Select,C179:H179)</f>
-        <v>-32895695.418253522</v>
+        <v>-14611060.229661105</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -13196,23 +13236,23 @@
       </c>
       <c r="E180" s="135">
         <f>E$172-E$152</f>
-        <v>20493175.167810693</v>
+        <v>22770194.630900763</v>
       </c>
       <c r="F180" s="135">
         <f>F$172-F$152</f>
-        <v>16500869.642468236</v>
+        <v>20371444.003047206</v>
       </c>
       <c r="G180" s="135">
         <f>G$172-G$152</f>
-        <v>13409088.395061092</v>
+        <v>18393811.241510414</v>
       </c>
       <c r="H180" s="135">
         <f>H$172-H$152</f>
-        <v>11054962.135826817</v>
+        <v>16849507.90401892</v>
       </c>
       <c r="I180" s="164">
         <f>SUM(C180:H180)</f>
-        <v>-25035470.882121891</v>
+        <v>-8108608.4438114278</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
les bonnes petites amélioration
</commit_message>
<xml_diff>
--- a/annexe/Modèle investissement.xlsx
+++ b/annexe/Modèle investissement.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927F8362-3E65-4BC3-BFDA-B9D0FD4B2E1E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F61DD57-7D49-4AB1-8FBC-017BA640774C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="2" r:id="rId1"/>
@@ -2525,38 +2525,38 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="39" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2966,19 +2966,19 @@
       <c r="B3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E3" s="226" t="s">
+      <c r="E3" s="224" t="s">
         <v>315</v>
       </c>
-      <c r="F3" s="227"/>
-      <c r="G3" s="228"/>
-      <c r="H3" s="224" t="s">
+      <c r="F3" s="225"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="222" t="s">
         <v>323</v>
       </c>
-      <c r="I3" s="225"/>
-      <c r="J3" s="224" t="s">
+      <c r="I3" s="223"/>
+      <c r="J3" s="222" t="s">
         <v>324</v>
       </c>
-      <c r="K3" s="225"/>
+      <c r="K3" s="223"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D4" s="190"/>
@@ -3056,19 +3056,19 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F69&lt;&gt;"",Select!G69&lt;&gt;""),Select!E69,""))</f>
         <v/>
       </c>
-      <c r="H6" s="229">
+      <c r="H6" s="227">
         <f>Modèle!D164</f>
         <v>0.11649484536082488</v>
       </c>
-      <c r="I6" s="231">
+      <c r="I6" s="229">
         <f>Modèle!I164</f>
         <v>0.5297697407485138</v>
       </c>
-      <c r="J6" s="229">
+      <c r="J6" s="227">
         <f>Modèle!D192</f>
         <v>0</v>
       </c>
-      <c r="K6" s="231">
+      <c r="K6" s="229">
         <f>Modèle!H192</f>
         <v>0.40232466137854034</v>
       </c>
@@ -3097,10 +3097,10 @@
         <f>IF(_Regime_Select=_Regime_Gen,"",IF(OR(Select!F70&lt;&gt;"",Select!G70&lt;&gt;""),Select!E70,""))</f>
         <v/>
       </c>
-      <c r="H7" s="230"/>
-      <c r="I7" s="232"/>
-      <c r="J7" s="230"/>
-      <c r="K7" s="232"/>
+      <c r="H7" s="228"/>
+      <c r="I7" s="230"/>
+      <c r="J7" s="228"/>
+      <c r="K7" s="230"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D8" s="56" t="str">
@@ -3249,15 +3249,15 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="222" t="str">
+      <c r="A16" s="231" t="str">
         <f>VLOOKUP(_Bilan,_Tables,4,FALSE)</f>
         <v>Bilan à l'ouverture</v>
       </c>
-      <c r="B16" s="222"/>
-      <c r="C16" s="222"/>
-      <c r="D16" s="222"/>
-      <c r="E16" s="222"/>
-      <c r="F16" s="222"/>
+      <c r="B16" s="231"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="231"/>
+      <c r="F16" s="231"/>
       <c r="H16" s="73" t="str">
         <f>VLOOKUP(_PIBPNB,_Tables,4,FALSE)</f>
         <v>PIB ou PNB</v>
@@ -3267,18 +3267,18 @@
       <c r="K16" s="68"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="223" t="str">
+      <c r="A17" s="232" t="str">
         <f>VLOOKUP(_Actif,_Tables,4,FALSE)</f>
         <v>Actif</v>
       </c>
-      <c r="B17" s="223"/>
-      <c r="C17" s="223"/>
-      <c r="D17" s="223" t="str">
+      <c r="B17" s="232"/>
+      <c r="C17" s="232"/>
+      <c r="D17" s="232" t="str">
         <f>VLOOKUP(_Passif,_Tables,4,FALSE)</f>
         <v>Passif</v>
       </c>
-      <c r="E17" s="223"/>
-      <c r="F17" s="223"/>
+      <c r="E17" s="232"/>
+      <c r="F17" s="232"/>
       <c r="H17" s="56" t="str">
         <f>_PIBPNB_Liste</f>
         <v>PIB/tête</v>
@@ -3587,29 +3587,29 @@
       <c r="K29" s="70"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="222" t="str">
+      <c r="A31" s="231" t="str">
         <f>VLOOKUP(_CompteDeResultat,_Tables,4,FALSE)</f>
         <v>Compte de résultat</v>
       </c>
-      <c r="B31" s="222"/>
-      <c r="C31" s="222"/>
-      <c r="D31" s="222"/>
-      <c r="E31" s="222"/>
-      <c r="F31" s="222"/>
+      <c r="B31" s="231"/>
+      <c r="C31" s="231"/>
+      <c r="D31" s="231"/>
+      <c r="E31" s="231"/>
+      <c r="F31" s="231"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="223" t="str">
+      <c r="A32" s="232" t="str">
         <f>VLOOKUP(_Charges,_Tables,4,FALSE)</f>
         <v>Charges</v>
       </c>
-      <c r="B32" s="223"/>
-      <c r="C32" s="223"/>
-      <c r="D32" s="223" t="str">
+      <c r="B32" s="232"/>
+      <c r="C32" s="232"/>
+      <c r="D32" s="232" t="str">
         <f>VLOOKUP(_Produits,_Tables,4,FALSE)</f>
         <v>Produits</v>
       </c>
-      <c r="E32" s="223"/>
-      <c r="F32" s="223"/>
+      <c r="E32" s="232"/>
+      <c r="F32" s="232"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="str">
@@ -4125,6 +4125,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E3:G3"/>
@@ -4132,12 +4138,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7189,10 +7189,10 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9078,10 +9078,10 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9514,10 +9514,10 @@
   <dimension ref="A1:Q209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E73" sqref="E73"/>
+      <selection pane="bottomRight" activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12907,7 +12907,7 @@
         <v>0.332926465850516</v>
       </c>
       <c r="I161" s="171">
-        <f t="shared" si="86"/>
+        <f>I145/I$171</f>
         <v>0.73720945141061001</v>
       </c>
       <c r="J161" s="216">
@@ -13878,7 +13878,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>